<commit_message>
co len co len co len
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
+++ b/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DE85BB-D82B-4E4D-94BF-F3F5E5D0078F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DA9B9-115E-407D-84C1-BAC4206EE5D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="600" firstSheet="6" activeTab="15" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="600" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
   <sheets>
     <sheet name="study plan" sheetId="22" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="899">
   <si>
     <t>No</t>
   </si>
@@ -2947,40 +2947,25 @@
     <t>lưu ý: leveling resource kỹ thuật. Sư dụng monte carlo để simulate. Monte carlo là dạng what if analysis</t>
   </si>
   <si>
-    <t>Stakeholder Area + exam</t>
-  </si>
-  <si>
-    <t>Procurement + Exam</t>
-  </si>
-  <si>
-    <t>Risk + Exam</t>
-  </si>
-  <si>
-    <t>Communication + Exam</t>
-  </si>
-  <si>
-    <t>Resource + Exam</t>
-  </si>
-  <si>
-    <t>Quality + Exam</t>
-  </si>
-  <si>
-    <t>Cost + Exam</t>
-  </si>
-  <si>
-    <t>Schedule + Exam</t>
-  </si>
-  <si>
-    <t>Scope + Exam</t>
-  </si>
-  <si>
-    <t>Intergrated + Exam</t>
-  </si>
-  <si>
-    <t>FW Project Management</t>
-  </si>
-  <si>
     <t>GOAL</t>
+  </si>
+  <si>
+    <t>Với yêu cầu phải reponse trước với new schedule khi thay đổi thì chỉ có sử dụng simulation technique such as monte carlo analysis để giả lập, tính toán cho total project. =&gt; cái này cần phải lựa chọn trước những option khác</t>
+  </si>
+  <si>
+    <t>Monitoring Process + exam</t>
+  </si>
+  <si>
+    <t>Executing process + Exam</t>
+  </si>
+  <si>
+    <t>Planning process + Exam</t>
+  </si>
+  <si>
+    <t>Initiating Process + Exam</t>
+  </si>
+  <si>
+    <t>Closing process + Exam</t>
   </si>
 </sst>
 </file>
@@ -3124,7 +3109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3183,6 +3168,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3535,7 +3526,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3884,6 +3875,21 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="11" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="17" fillId="11" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4286,13 +4292,13 @@
   </sheetPr>
   <dimension ref="A1:AA1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.42578125" style="57"/>
     <col min="6" max="9" width="14.42578125" style="56"/>
     <col min="10" max="16384" width="14.42578125" style="57"/>
@@ -4318,7 +4324,7 @@
         <v>578</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>903</v>
+        <v>892</v>
       </c>
       <c r="H1" s="60" t="s">
         <v>459</v>
@@ -5432,7 +5438,7 @@
       <c r="Z27" s="56"/>
       <c r="AA27" s="56"/>
     </row>
-    <row r="28" spans="1:27" ht="15">
+    <row r="28" spans="1:27" ht="15.75" thickBot="1">
       <c r="A28" s="109" t="s">
         <v>396</v>
       </c>
@@ -5477,20 +5483,20 @@
       <c r="AA28" s="56"/>
     </row>
     <row r="29" spans="1:27" ht="15">
-      <c r="A29" s="115" t="s">
-        <v>892</v>
-      </c>
-      <c r="B29" s="116">
+      <c r="A29" s="129" t="s">
+        <v>894</v>
+      </c>
+      <c r="B29" s="130">
         <v>43493</v>
       </c>
-      <c r="C29" s="116" t="str">
+      <c r="C29" s="130" t="str">
         <f>IF(WEEKDAY(B29,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B29,1))</f>
         <v>Thứ 2</v>
       </c>
-      <c r="D29" s="117">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E29" s="118"/>
+      <c r="D29" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E29" s="132"/>
       <c r="F29" s="119"/>
       <c r="G29" s="119"/>
       <c r="H29" s="119"/>
@@ -5603,7 +5609,7 @@
       <c r="Z31" s="56"/>
       <c r="AA31" s="56"/>
     </row>
-    <row r="32" spans="1:27" ht="15">
+    <row r="32" spans="1:27" ht="15.75" thickBot="1">
       <c r="A32" s="115" t="s">
         <v>361</v>
       </c>
@@ -5649,21 +5655,21 @@
       <c r="AA32" s="56"/>
     </row>
     <row r="33" spans="1:27" ht="15">
-      <c r="A33" s="115" t="s">
-        <v>893</v>
-      </c>
-      <c r="B33" s="116">
+      <c r="A33" s="129" t="s">
+        <v>895</v>
+      </c>
+      <c r="B33" s="130">
         <f>B30+ 1</f>
         <v>43494</v>
       </c>
-      <c r="C33" s="116" t="str">
+      <c r="C33" s="130" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D33" s="117">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E33" s="118"/>
+      <c r="D33" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E33" s="132"/>
       <c r="F33" s="119"/>
       <c r="G33" s="119"/>
       <c r="H33" s="119"/>
@@ -5730,7 +5736,7 @@
       <c r="Z34" s="56"/>
       <c r="AA34" s="56"/>
     </row>
-    <row r="35" spans="1:27" ht="15">
+    <row r="35" spans="1:27" ht="15.75" thickBot="1">
       <c r="A35" s="121" t="s">
         <v>372</v>
       </c>
@@ -5776,21 +5782,21 @@
       <c r="AA35" s="56"/>
     </row>
     <row r="36" spans="1:27" ht="15">
-      <c r="A36" s="121" t="s">
-        <v>894</v>
-      </c>
-      <c r="B36" s="116">
+      <c r="A36" s="133" t="s">
+        <v>896</v>
+      </c>
+      <c r="B36" s="130">
         <f>B30 + 2</f>
         <v>43495</v>
       </c>
-      <c r="C36" s="116" t="str">
+      <c r="C36" s="130" t="str">
         <f t="shared" si="5"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D36" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E36" s="118"/>
+      <c r="D36" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E36" s="132"/>
       <c r="F36" s="119"/>
       <c r="G36" s="119"/>
       <c r="H36" s="119"/>
@@ -5859,7 +5865,7 @@
       <c r="Z37" s="56"/>
       <c r="AA37" s="56"/>
     </row>
-    <row r="38" spans="1:27" ht="15">
+    <row r="38" spans="1:27" ht="15.75" thickBot="1">
       <c r="A38" s="121" t="s">
         <v>364</v>
       </c>
@@ -5903,21 +5909,21 @@
       <c r="AA38" s="56"/>
     </row>
     <row r="39" spans="1:27" ht="15">
-      <c r="A39" s="121" t="s">
-        <v>895</v>
-      </c>
-      <c r="B39" s="116">
+      <c r="A39" s="133" t="s">
+        <v>897</v>
+      </c>
+      <c r="B39" s="130">
         <f>B36 + 1</f>
         <v>43496</v>
       </c>
-      <c r="C39" s="116" t="str">
+      <c r="C39" s="130" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D39" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E39" s="117"/>
+      <c r="D39" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E39" s="132"/>
       <c r="F39" s="119"/>
       <c r="G39" s="119"/>
       <c r="H39" s="119"/>
@@ -5986,7 +5992,7 @@
       <c r="Z40" s="56"/>
       <c r="AA40" s="56"/>
     </row>
-    <row r="41" spans="1:27" ht="15">
+    <row r="41" spans="1:27" ht="15.75" thickBot="1">
       <c r="A41" s="115" t="s">
         <v>402</v>
       </c>
@@ -6032,21 +6038,21 @@
       <c r="AA41" s="56"/>
     </row>
     <row r="42" spans="1:27" ht="15">
-      <c r="A42" s="115" t="s">
-        <v>896</v>
-      </c>
-      <c r="B42" s="116">
+      <c r="A42" s="133" t="s">
+        <v>898</v>
+      </c>
+      <c r="B42" s="130">
         <f>B39 + 1</f>
         <v>43497</v>
       </c>
-      <c r="C42" s="116" t="str">
+      <c r="C42" s="130" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D42" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E42" s="118"/>
+      <c r="D42" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E42" s="132"/>
       <c r="F42" s="119"/>
       <c r="G42" s="119"/>
       <c r="H42" s="119"/>
@@ -6113,7 +6119,7 @@
       <c r="Z43" s="56"/>
       <c r="AA43" s="56"/>
     </row>
-    <row r="44" spans="1:27" ht="15">
+    <row r="44" spans="1:27" ht="15.75" thickBot="1">
       <c r="A44" s="115" t="s">
         <v>365</v>
       </c>
@@ -6159,21 +6165,21 @@
       <c r="AA44" s="56"/>
     </row>
     <row r="45" spans="1:27" ht="15">
-      <c r="A45" s="115" t="s">
+      <c r="A45" s="133" t="s">
         <v>897</v>
       </c>
-      <c r="B45" s="116">
+      <c r="B45" s="130">
         <f>B38+ 2</f>
         <v>43498</v>
       </c>
-      <c r="C45" s="116" t="str">
+      <c r="C45" s="130" t="str">
         <f t="shared" si="6"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D45" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E45" s="118"/>
+      <c r="D45" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E45" s="132"/>
       <c r="F45" s="119"/>
       <c r="G45" s="119"/>
       <c r="H45" s="119"/>
@@ -6240,7 +6246,7 @@
       <c r="Z46" s="56"/>
       <c r="AA46" s="56"/>
     </row>
-    <row r="47" spans="1:27" ht="15">
+    <row r="47" spans="1:27" ht="15.75" thickBot="1">
       <c r="A47" s="115" t="s">
         <v>403</v>
       </c>
@@ -6280,21 +6286,21 @@
       <c r="AA47" s="56"/>
     </row>
     <row r="48" spans="1:27" ht="15">
-      <c r="A48" s="115" t="s">
-        <v>898</v>
-      </c>
-      <c r="B48" s="128">
+      <c r="A48" s="133" t="s">
+        <v>896</v>
+      </c>
+      <c r="B48" s="130">
         <f>B45+1</f>
         <v>43499</v>
       </c>
-      <c r="C48" s="116" t="str">
+      <c r="C48" s="130" t="str">
         <f t="shared" si="6"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D48" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E48" s="118"/>
+      <c r="D48" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E48" s="132"/>
       <c r="F48" s="119"/>
       <c r="G48" s="119"/>
       <c r="H48" s="119"/>
@@ -6357,7 +6363,7 @@
       <c r="Z49" s="56"/>
       <c r="AA49" s="56"/>
     </row>
-    <row r="50" spans="1:27" ht="15">
+    <row r="50" spans="1:27" ht="15.75" thickBot="1">
       <c r="A50" s="115" t="s">
         <v>374</v>
       </c>
@@ -6397,21 +6403,21 @@
       <c r="AA50" s="56"/>
     </row>
     <row r="51" spans="1:27" ht="15">
-      <c r="A51" s="115" t="s">
-        <v>899</v>
-      </c>
-      <c r="B51" s="116">
+      <c r="A51" s="133" t="s">
+        <v>895</v>
+      </c>
+      <c r="B51" s="130">
         <f>B45 + 2</f>
         <v>43500</v>
       </c>
-      <c r="C51" s="116" t="str">
+      <c r="C51" s="130" t="str">
         <f t="shared" si="7"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D51" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E51" s="118"/>
+      <c r="D51" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E51" s="132"/>
       <c r="F51" s="119"/>
       <c r="G51" s="119"/>
       <c r="H51" s="119"/>
@@ -6474,7 +6480,7 @@
       <c r="Z52" s="56"/>
       <c r="AA52" s="56"/>
     </row>
-    <row r="53" spans="1:27" ht="15">
+    <row r="53" spans="1:27" ht="15.75" thickBot="1">
       <c r="A53" s="115" t="s">
         <v>368</v>
       </c>
@@ -6514,21 +6520,21 @@
       <c r="AA53" s="56"/>
     </row>
     <row r="54" spans="1:27" ht="15">
-      <c r="A54" s="115" t="s">
-        <v>900</v>
-      </c>
-      <c r="B54" s="128">
+      <c r="A54" s="133" t="s">
+        <v>898</v>
+      </c>
+      <c r="B54" s="130">
         <f>B45+3</f>
         <v>43501</v>
       </c>
-      <c r="C54" s="116" t="str">
+      <c r="C54" s="130" t="str">
         <f t="shared" si="7"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D54" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E54" s="118"/>
+      <c r="D54" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E54" s="132"/>
       <c r="F54" s="119"/>
       <c r="G54" s="119"/>
       <c r="H54" s="119"/>
@@ -6591,7 +6597,7 @@
       <c r="Z55" s="56"/>
       <c r="AA55" s="56"/>
     </row>
-    <row r="56" spans="1:27" ht="15">
+    <row r="56" spans="1:27" ht="15.75" thickBot="1">
       <c r="A56" s="115" t="s">
         <v>406</v>
       </c>
@@ -6631,21 +6637,21 @@
       <c r="AA56" s="56"/>
     </row>
     <row r="57" spans="1:27" ht="15">
-      <c r="A57" s="115" t="s">
-        <v>901</v>
-      </c>
-      <c r="B57" s="116">
+      <c r="A57" s="133" t="s">
+        <v>894</v>
+      </c>
+      <c r="B57" s="130">
         <f>B54 + 1</f>
         <v>43502</v>
       </c>
-      <c r="C57" s="116" t="str">
+      <c r="C57" s="130" t="str">
         <f t="shared" si="7"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D57" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E57" s="118"/>
+      <c r="D57" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E57" s="132"/>
       <c r="F57" s="119"/>
       <c r="G57" s="119"/>
       <c r="H57" s="119"/>
@@ -6708,7 +6714,7 @@
       <c r="Z58" s="56"/>
       <c r="AA58" s="56"/>
     </row>
-    <row r="59" spans="1:27" ht="15">
+    <row r="59" spans="1:27" ht="15.75" thickBot="1">
       <c r="A59" s="115" t="s">
         <v>376</v>
       </c>
@@ -6748,21 +6754,21 @@
       <c r="AA59" s="56"/>
     </row>
     <row r="60" spans="1:27" ht="15">
-      <c r="A60" s="115" t="s">
-        <v>902</v>
-      </c>
-      <c r="B60" s="116">
+      <c r="A60" s="133" t="s">
+        <v>895</v>
+      </c>
+      <c r="B60" s="130">
         <f>B57 + 1</f>
         <v>43503</v>
       </c>
-      <c r="C60" s="116" t="str">
+      <c r="C60" s="130" t="str">
         <f t="shared" si="8"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D60" s="117">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E60" s="118"/>
+      <c r="D60" s="131">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E60" s="132"/>
       <c r="F60" s="119"/>
       <c r="G60" s="119"/>
       <c r="H60" s="119"/>
@@ -34313,8 +34319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AD6CE4-A652-4BA6-AF5B-7B55F9607709}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34423,14 +34429,18 @@
       <c r="F7" s="76"/>
       <c r="G7" s="77"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="90">
       <c r="A8" s="72">
         <v>7</v>
       </c>
       <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="C8" s="72" t="s">
+        <v>4</v>
+      </c>
       <c r="D8" s="72"/>
-      <c r="E8" s="75"/>
+      <c r="E8" s="75" t="s">
+        <v>893</v>
+      </c>
       <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:8">

</xml_diff>

<commit_message>
co len khong de cham deadline nua
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
+++ b/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DA9B9-115E-407D-84C1-BAC4206EE5D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42BC3F1-CB89-4222-86D9-7FD9E20352B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="600" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="600" firstSheet="10" activeTab="15" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
   <sheets>
     <sheet name="study plan" sheetId="22" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="900">
   <si>
     <t>No</t>
   </si>
@@ -2966,6 +2966,9 @@
   </si>
   <si>
     <t>Closing process + Exam</t>
+  </si>
+  <si>
+    <t>Milestones significant (đánh dấu) events within the project schedule. Chúng k phải là work activities. They have no duration</t>
   </si>
 </sst>
 </file>
@@ -3774,28 +3777,6 @@
     <xf numFmtId="14" fontId="13" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3890,6 +3871,28 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4292,8 +4295,8 @@
   </sheetPr>
   <dimension ref="A1:AA1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -4904,10 +4907,10 @@
       <c r="A15" s="84" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="93">
+      <c r="B15" s="126">
         <v>43473</v>
       </c>
-      <c r="C15" s="93" t="str">
+      <c r="C15" s="126" t="str">
         <f t="shared" si="1"/>
         <v>Thứ 3</v>
       </c>
@@ -4948,8 +4951,8 @@
       <c r="A16" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
+      <c r="B16" s="127"/>
+      <c r="C16" s="127"/>
       <c r="D16" s="79">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -4987,8 +4990,8 @@
       <c r="A17" s="84" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="94"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="127"/>
       <c r="D17" s="79">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5067,26 +5070,26 @@
       <c r="AA18" s="56"/>
     </row>
     <row r="19" spans="1:27" ht="15">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="94" t="s">
         <v>396</v>
       </c>
-      <c r="B19" s="103">
+      <c r="B19" s="95">
         <v>43478</v>
       </c>
-      <c r="C19" s="103" t="str">
+      <c r="C19" s="95" t="str">
         <f t="shared" si="2"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D19" s="104">
+      <c r="D19" s="96">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E19" s="105"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106" t="s">
+      <c r="E19" s="97"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98" t="s">
         <v>473</v>
       </c>
-      <c r="I19" s="106" t="s">
+      <c r="I19" s="98" t="s">
         <v>549</v>
       </c>
       <c r="J19" s="56"/>
@@ -5112,11 +5115,11 @@
       <c r="A20" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="B20" s="93">
+      <c r="B20" s="126">
         <f>B19+1</f>
         <v>43479</v>
       </c>
-      <c r="C20" s="93" t="str">
+      <c r="C20" s="126" t="str">
         <f t="shared" si="2"/>
         <v>Thứ 2</v>
       </c>
@@ -5157,8 +5160,8 @@
       <c r="A21" s="84" t="s">
         <v>359</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
+      <c r="B21" s="127"/>
+      <c r="C21" s="127"/>
       <c r="D21" s="79">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5194,8 +5197,8 @@
       <c r="A22" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
+      <c r="B22" s="127"/>
+      <c r="C22" s="127"/>
       <c r="D22" s="79">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -5275,27 +5278,27 @@
       <c r="AA23" s="56"/>
     </row>
     <row r="24" spans="1:27" ht="15">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="99" t="s">
         <v>398</v>
       </c>
-      <c r="B24" s="103">
+      <c r="B24" s="95">
         <f>B20 + 1</f>
         <v>43480</v>
       </c>
-      <c r="C24" s="103" t="str">
+      <c r="C24" s="95" t="str">
         <f t="shared" si="3"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D24" s="104">
+      <c r="D24" s="96">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E24" s="105"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="106"/>
-      <c r="H24" s="106" t="s">
+      <c r="E24" s="97"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98" t="s">
         <v>478</v>
       </c>
-      <c r="I24" s="106" t="s">
+      <c r="I24" s="98" t="s">
         <v>549</v>
       </c>
       <c r="J24" s="56"/>
@@ -5363,21 +5366,21 @@
       <c r="AA25" s="56"/>
     </row>
     <row r="26" spans="1:27" ht="15">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="99" t="s">
         <v>361</v>
       </c>
-      <c r="B26" s="108"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="104">
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="96">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E26" s="105"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106" t="s">
+      <c r="E26" s="97"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98" t="s">
         <v>480</v>
       </c>
-      <c r="I26" s="106" t="s">
+      <c r="I26" s="98" t="s">
         <v>860</v>
       </c>
       <c r="J26" s="56"/>
@@ -5439,28 +5442,28 @@
       <c r="AA27" s="56"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A28" s="109" t="s">
+      <c r="A28" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="B28" s="110">
+      <c r="B28" s="102">
         <v>43493</v>
       </c>
-      <c r="C28" s="110" t="str">
+      <c r="C28" s="102" t="str">
         <f>IF(WEEKDAY(B28,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B28,1))</f>
         <v>Thứ 2</v>
       </c>
-      <c r="D28" s="111">
+      <c r="D28" s="103">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E28" s="112"/>
-      <c r="F28" s="113" t="s">
+      <c r="E28" s="104"/>
+      <c r="F28" s="105" t="s">
         <v>788</v>
       </c>
-      <c r="G28" s="113"/>
-      <c r="H28" s="113" t="s">
+      <c r="G28" s="105"/>
+      <c r="H28" s="105" t="s">
         <v>473</v>
       </c>
-      <c r="I28" s="114" t="s">
+      <c r="I28" s="106" t="s">
         <v>549</v>
       </c>
       <c r="J28" s="56"/>
@@ -5483,24 +5486,24 @@
       <c r="AA28" s="56"/>
     </row>
     <row r="29" spans="1:27" ht="15">
-      <c r="A29" s="129" t="s">
+      <c r="A29" s="121" t="s">
         <v>894</v>
       </c>
-      <c r="B29" s="130">
+      <c r="B29" s="122">
         <v>43493</v>
       </c>
-      <c r="C29" s="130" t="str">
+      <c r="C29" s="122" t="str">
         <f>IF(WEEKDAY(B29,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B29,1))</f>
         <v>Thứ 2</v>
       </c>
-      <c r="D29" s="131">
+      <c r="D29" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E29" s="132"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="119"/>
-      <c r="I29" s="120"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="112"/>
       <c r="J29" s="56"/>
       <c r="K29" s="56"/>
       <c r="L29" s="56"/>
@@ -5521,28 +5524,28 @@
       <c r="AA29" s="56"/>
     </row>
     <row r="30" spans="1:27" ht="15">
-      <c r="A30" s="115" t="s">
+      <c r="A30" s="107" t="s">
         <v>399</v>
       </c>
-      <c r="B30" s="116">
+      <c r="B30" s="108">
         <v>43493</v>
       </c>
-      <c r="C30" s="116" t="str">
+      <c r="C30" s="108" t="str">
         <f t="shared" ref="C30:C42" si="4">IF(WEEKDAY(B30,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B30,1))</f>
         <v>Thứ 2</v>
       </c>
-      <c r="D30" s="117">
+      <c r="D30" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E30" s="118"/>
-      <c r="F30" s="119" t="s">
+      <c r="E30" s="110"/>
+      <c r="F30" s="111" t="s">
         <v>788</v>
       </c>
-      <c r="G30" s="119"/>
-      <c r="H30" s="119" t="s">
+      <c r="G30" s="111"/>
+      <c r="H30" s="111" t="s">
         <v>482</v>
       </c>
-      <c r="I30" s="120" t="s">
+      <c r="I30" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J30" s="56"/>
@@ -5565,29 +5568,29 @@
       <c r="AA30" s="56"/>
     </row>
     <row r="31" spans="1:27" ht="15">
-      <c r="A31" s="115" t="s">
+      <c r="A31" s="107" t="s">
         <v>398</v>
       </c>
-      <c r="B31" s="116">
+      <c r="B31" s="108">
         <f>B28+ 1</f>
         <v>43494</v>
       </c>
-      <c r="C31" s="116" t="str">
+      <c r="C31" s="108" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D31" s="117">
+      <c r="D31" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E31" s="118"/>
-      <c r="F31" s="119" t="s">
+      <c r="E31" s="110"/>
+      <c r="F31" s="111" t="s">
         <v>788</v>
       </c>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119" t="s">
+      <c r="G31" s="111"/>
+      <c r="H31" s="111" t="s">
         <v>478</v>
       </c>
-      <c r="I31" s="120" t="s">
+      <c r="I31" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J31" s="56"/>
@@ -5610,29 +5613,29 @@
       <c r="AA31" s="56"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="107" t="s">
         <v>361</v>
       </c>
-      <c r="B32" s="116">
+      <c r="B32" s="108">
         <f>B29+ 1</f>
         <v>43494</v>
       </c>
-      <c r="C32" s="116" t="str">
+      <c r="C32" s="108" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D32" s="117">
+      <c r="D32" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E32" s="118"/>
-      <c r="F32" s="119" t="s">
+      <c r="E32" s="110"/>
+      <c r="F32" s="111" t="s">
         <v>788</v>
       </c>
-      <c r="G32" s="119"/>
-      <c r="H32" s="119" t="s">
+      <c r="G32" s="111"/>
+      <c r="H32" s="111" t="s">
         <v>480</v>
       </c>
-      <c r="I32" s="120" t="s">
+      <c r="I32" s="112" t="s">
         <v>860</v>
       </c>
       <c r="J32" s="56"/>
@@ -5655,25 +5658,25 @@
       <c r="AA32" s="56"/>
     </row>
     <row r="33" spans="1:27" ht="15">
-      <c r="A33" s="129" t="s">
+      <c r="A33" s="121" t="s">
         <v>895</v>
       </c>
-      <c r="B33" s="130">
+      <c r="B33" s="122">
         <f>B30+ 1</f>
         <v>43494</v>
       </c>
-      <c r="C33" s="130" t="str">
+      <c r="C33" s="122" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D33" s="131">
+      <c r="D33" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E33" s="132"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="119"/>
-      <c r="I33" s="120"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="112"/>
       <c r="J33" s="56"/>
       <c r="K33" s="56"/>
       <c r="L33" s="56"/>
@@ -5694,29 +5697,29 @@
       <c r="AA33" s="56"/>
     </row>
     <row r="34" spans="1:27" ht="15">
-      <c r="A34" s="115" t="s">
+      <c r="A34" s="107" t="s">
         <v>400</v>
       </c>
-      <c r="B34" s="116">
+      <c r="B34" s="108">
         <f>B28 + 2</f>
         <v>43495</v>
       </c>
-      <c r="C34" s="116" t="str">
+      <c r="C34" s="108" t="str">
         <f>IF(WEEKDAY(B34,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B34,1))</f>
         <v>Thứ 4</v>
       </c>
-      <c r="D34" s="117">
+      <c r="D34" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E34" s="118"/>
-      <c r="F34" s="119" t="s">
+      <c r="E34" s="110"/>
+      <c r="F34" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119" t="s">
+      <c r="G34" s="111"/>
+      <c r="H34" s="111" t="s">
         <v>483</v>
       </c>
-      <c r="I34" s="120"/>
+      <c r="I34" s="112"/>
       <c r="J34" s="56"/>
       <c r="K34" s="56"/>
       <c r="L34" s="56"/>
@@ -5737,29 +5740,29 @@
       <c r="AA34" s="56"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A35" s="121" t="s">
+      <c r="A35" s="113" t="s">
         <v>372</v>
       </c>
-      <c r="B35" s="116">
+      <c r="B35" s="108">
         <f>B29 + 2</f>
         <v>43495</v>
       </c>
-      <c r="C35" s="116" t="str">
+      <c r="C35" s="108" t="str">
         <f t="shared" ref="C35:C36" si="5">IF(WEEKDAY(B35,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B35,1))</f>
         <v>Thứ 4</v>
       </c>
-      <c r="D35" s="117">
+      <c r="D35" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E35" s="118"/>
-      <c r="F35" s="119" t="s">
+      <c r="E35" s="110"/>
+      <c r="F35" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G35" s="119"/>
-      <c r="H35" s="119" t="s">
+      <c r="G35" s="111"/>
+      <c r="H35" s="111" t="s">
         <v>484</v>
       </c>
-      <c r="I35" s="120" t="s">
+      <c r="I35" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J35" s="56"/>
@@ -5782,25 +5785,25 @@
       <c r="AA35" s="56"/>
     </row>
     <row r="36" spans="1:27" ht="15">
-      <c r="A36" s="133" t="s">
+      <c r="A36" s="125" t="s">
         <v>896</v>
       </c>
-      <c r="B36" s="130">
+      <c r="B36" s="122">
         <f>B30 + 2</f>
         <v>43495</v>
       </c>
-      <c r="C36" s="130" t="str">
+      <c r="C36" s="122" t="str">
         <f t="shared" si="5"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D36" s="131">
+      <c r="D36" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E36" s="132"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="120"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="111"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="112"/>
       <c r="J36" s="56"/>
       <c r="K36" s="56"/>
       <c r="L36" s="56"/>
@@ -5821,29 +5824,29 @@
       <c r="AA36" s="56"/>
     </row>
     <row r="37" spans="1:27" ht="15">
-      <c r="A37" s="115" t="s">
+      <c r="A37" s="107" t="s">
         <v>363</v>
       </c>
-      <c r="B37" s="116">
-        <f>B34 + 1</f>
+      <c r="B37" s="108">
+        <f t="shared" ref="B37:B42" si="6">B34 + 1</f>
         <v>43496</v>
       </c>
-      <c r="C37" s="116" t="str">
+      <c r="C37" s="108" t="str">
         <f>IF(WEEKDAY(B37,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B37,1))</f>
         <v>Thứ 5</v>
       </c>
-      <c r="D37" s="117">
+      <c r="D37" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E37" s="118"/>
-      <c r="F37" s="119" t="s">
+      <c r="E37" s="110"/>
+      <c r="F37" s="111" t="s">
         <v>788</v>
       </c>
-      <c r="G37" s="119"/>
-      <c r="H37" s="119" t="s">
+      <c r="G37" s="111"/>
+      <c r="H37" s="111" t="s">
         <v>485</v>
       </c>
-      <c r="I37" s="120" t="s">
+      <c r="I37" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J37" s="56"/>
@@ -5866,27 +5869,27 @@
       <c r="AA37" s="56"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A38" s="121" t="s">
+      <c r="A38" s="113" t="s">
         <v>364</v>
       </c>
-      <c r="B38" s="116">
-        <f>B35 + 1</f>
+      <c r="B38" s="108">
+        <f t="shared" si="6"/>
         <v>43496</v>
       </c>
-      <c r="C38" s="116" t="str">
+      <c r="C38" s="108" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D38" s="117">
+      <c r="D38" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E38" s="117"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119" t="s">
+      <c r="E38" s="109"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111" t="s">
         <v>486</v>
       </c>
-      <c r="I38" s="120" t="s">
+      <c r="I38" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J38" s="56"/>
@@ -5909,25 +5912,25 @@
       <c r="AA38" s="56"/>
     </row>
     <row r="39" spans="1:27" ht="15">
-      <c r="A39" s="133" t="s">
+      <c r="A39" s="125" t="s">
         <v>897</v>
       </c>
-      <c r="B39" s="130">
-        <f>B36 + 1</f>
+      <c r="B39" s="122">
+        <f t="shared" si="6"/>
         <v>43496</v>
       </c>
-      <c r="C39" s="130" t="str">
+      <c r="C39" s="122" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D39" s="131">
+      <c r="D39" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E39" s="132"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="120"/>
+      <c r="E39" s="124"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111"/>
+      <c r="H39" s="111"/>
+      <c r="I39" s="112"/>
       <c r="J39" s="56"/>
       <c r="K39" s="56"/>
       <c r="L39" s="56"/>
@@ -5948,29 +5951,29 @@
       <c r="AA39" s="56"/>
     </row>
     <row r="40" spans="1:27" ht="15">
-      <c r="A40" s="115" t="s">
+      <c r="A40" s="107" t="s">
         <v>401</v>
       </c>
-      <c r="B40" s="116">
-        <f>B37 + 1</f>
+      <c r="B40" s="108">
+        <f t="shared" si="6"/>
         <v>43497</v>
       </c>
-      <c r="C40" s="116" t="str">
+      <c r="C40" s="108" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D40" s="117">
+      <c r="D40" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E40" s="118"/>
-      <c r="F40" s="119" t="s">
+      <c r="E40" s="110"/>
+      <c r="F40" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119" t="s">
+      <c r="G40" s="111"/>
+      <c r="H40" s="111" t="s">
         <v>487</v>
       </c>
-      <c r="I40" s="120" t="s">
+      <c r="I40" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J40" s="56"/>
@@ -5993,29 +5996,29 @@
       <c r="AA40" s="56"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A41" s="115" t="s">
+      <c r="A41" s="107" t="s">
         <v>402</v>
       </c>
-      <c r="B41" s="116">
-        <f>B38 + 1</f>
+      <c r="B41" s="108">
+        <f t="shared" si="6"/>
         <v>43497</v>
       </c>
-      <c r="C41" s="116" t="str">
+      <c r="C41" s="108" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D41" s="117">
+      <c r="D41" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E41" s="118"/>
-      <c r="F41" s="119" t="s">
+      <c r="E41" s="110"/>
+      <c r="F41" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G41" s="119"/>
-      <c r="H41" s="119" t="s">
+      <c r="G41" s="111"/>
+      <c r="H41" s="111" t="s">
         <v>488</v>
       </c>
-      <c r="I41" s="120" t="s">
+      <c r="I41" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J41" s="56"/>
@@ -6038,25 +6041,25 @@
       <c r="AA41" s="56"/>
     </row>
     <row r="42" spans="1:27" ht="15">
-      <c r="A42" s="133" t="s">
+      <c r="A42" s="125" t="s">
         <v>898</v>
       </c>
-      <c r="B42" s="130">
-        <f>B39 + 1</f>
+      <c r="B42" s="122">
+        <f t="shared" si="6"/>
         <v>43497</v>
       </c>
-      <c r="C42" s="130" t="str">
+      <c r="C42" s="122" t="str">
         <f t="shared" si="4"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D42" s="131">
+      <c r="D42" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E42" s="132"/>
-      <c r="F42" s="119"/>
-      <c r="G42" s="119"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="120"/>
+      <c r="E42" s="124"/>
+      <c r="F42" s="111"/>
+      <c r="G42" s="111"/>
+      <c r="H42" s="111"/>
+      <c r="I42" s="112"/>
       <c r="J42" s="56"/>
       <c r="K42" s="56"/>
       <c r="L42" s="56"/>
@@ -6077,29 +6080,29 @@
       <c r="AA42" s="56"/>
     </row>
     <row r="43" spans="1:27" ht="15">
-      <c r="A43" s="115" t="s">
+      <c r="A43" s="107" t="s">
         <v>373</v>
       </c>
-      <c r="B43" s="116">
+      <c r="B43" s="108">
         <f>B37+ 2</f>
         <v>43498</v>
       </c>
-      <c r="C43" s="116" t="str">
-        <f t="shared" ref="C43:C48" si="6">IF(WEEKDAY(B43,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B43,1))</f>
+      <c r="C43" s="108" t="str">
+        <f t="shared" ref="C43:C48" si="7">IF(WEEKDAY(B43,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B43,1))</f>
         <v>Thứ 7</v>
       </c>
-      <c r="D43" s="117">
+      <c r="D43" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E43" s="118"/>
-      <c r="F43" s="119" t="s">
+      <c r="E43" s="110"/>
+      <c r="F43" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G43" s="119"/>
-      <c r="H43" s="119" t="s">
+      <c r="G43" s="111"/>
+      <c r="H43" s="111" t="s">
         <v>489</v>
       </c>
-      <c r="I43" s="120"/>
+      <c r="I43" s="112"/>
       <c r="J43" s="56"/>
       <c r="K43" s="56"/>
       <c r="L43" s="56"/>
@@ -6120,29 +6123,29 @@
       <c r="AA43" s="56"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A44" s="115" t="s">
+      <c r="A44" s="107" t="s">
         <v>365</v>
       </c>
-      <c r="B44" s="116">
+      <c r="B44" s="108">
         <f>B37+ 2</f>
         <v>43498</v>
       </c>
-      <c r="C44" s="116" t="str">
-        <f t="shared" si="6"/>
+      <c r="C44" s="108" t="str">
+        <f t="shared" si="7"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D44" s="117">
+      <c r="D44" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E44" s="118"/>
-      <c r="F44" s="119" t="s">
+      <c r="E44" s="110"/>
+      <c r="F44" s="111" t="s">
         <v>577</v>
       </c>
-      <c r="G44" s="119"/>
-      <c r="H44" s="119" t="s">
+      <c r="G44" s="111"/>
+      <c r="H44" s="111" t="s">
         <v>490</v>
       </c>
-      <c r="I44" s="120" t="s">
+      <c r="I44" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J44" s="56"/>
@@ -6165,25 +6168,25 @@
       <c r="AA44" s="56"/>
     </row>
     <row r="45" spans="1:27" ht="15">
-      <c r="A45" s="133" t="s">
+      <c r="A45" s="125" t="s">
         <v>897</v>
       </c>
-      <c r="B45" s="130">
+      <c r="B45" s="122">
         <f>B38+ 2</f>
         <v>43498</v>
       </c>
-      <c r="C45" s="130" t="str">
-        <f t="shared" si="6"/>
+      <c r="C45" s="122" t="str">
+        <f t="shared" si="7"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D45" s="131">
+      <c r="D45" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E45" s="132"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="120"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="112"/>
       <c r="J45" s="56"/>
       <c r="K45" s="56"/>
       <c r="L45" s="56"/>
@@ -6204,27 +6207,27 @@
       <c r="AA45" s="56"/>
     </row>
     <row r="46" spans="1:27" ht="15">
-      <c r="A46" s="115" t="s">
+      <c r="A46" s="107" t="s">
         <v>366</v>
       </c>
-      <c r="B46" s="128">
+      <c r="B46" s="120">
         <f>B44+1</f>
         <v>43499</v>
       </c>
-      <c r="C46" s="116" t="str">
-        <f t="shared" si="6"/>
+      <c r="C46" s="108" t="str">
+        <f t="shared" si="7"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D46" s="117">
+      <c r="D46" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E46" s="118"/>
-      <c r="F46" s="119"/>
-      <c r="G46" s="119"/>
-      <c r="H46" s="119" t="s">
+      <c r="E46" s="110"/>
+      <c r="F46" s="111"/>
+      <c r="G46" s="111"/>
+      <c r="H46" s="111" t="s">
         <v>491</v>
       </c>
-      <c r="I46" s="120" t="s">
+      <c r="I46" s="112" t="s">
         <v>549</v>
       </c>
       <c r="J46" s="56"/>
@@ -6247,25 +6250,25 @@
       <c r="AA46" s="56"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A47" s="115" t="s">
+      <c r="A47" s="107" t="s">
         <v>403</v>
       </c>
-      <c r="B47" s="128">
+      <c r="B47" s="120">
         <f>B45+1</f>
         <v>43499</v>
       </c>
-      <c r="C47" s="116" t="str">
-        <f t="shared" si="6"/>
+      <c r="C47" s="108" t="str">
+        <f t="shared" si="7"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D47" s="117">
+      <c r="D47" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E47" s="118"/>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
-      <c r="I47" s="120"/>
+      <c r="E47" s="110"/>
+      <c r="F47" s="111"/>
+      <c r="G47" s="111"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="112"/>
       <c r="J47" s="56"/>
       <c r="K47" s="56"/>
       <c r="L47" s="56"/>
@@ -6286,25 +6289,25 @@
       <c r="AA47" s="56"/>
     </row>
     <row r="48" spans="1:27" ht="15">
-      <c r="A48" s="133" t="s">
+      <c r="A48" s="125" t="s">
         <v>896</v>
       </c>
-      <c r="B48" s="130">
+      <c r="B48" s="122">
         <f>B45+1</f>
         <v>43499</v>
       </c>
-      <c r="C48" s="130" t="str">
-        <f t="shared" si="6"/>
+      <c r="C48" s="122" t="str">
+        <f t="shared" si="7"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D48" s="131">
+      <c r="D48" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E48" s="132"/>
-      <c r="F48" s="119"/>
-      <c r="G48" s="119"/>
-      <c r="H48" s="119"/>
-      <c r="I48" s="120"/>
+      <c r="E48" s="124"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="112"/>
       <c r="J48" s="56"/>
       <c r="K48" s="56"/>
       <c r="L48" s="56"/>
@@ -6325,25 +6328,25 @@
       <c r="AA48" s="56"/>
     </row>
     <row r="49" spans="1:27" ht="15">
-      <c r="A49" s="115" t="s">
+      <c r="A49" s="107" t="s">
         <v>404</v>
       </c>
-      <c r="B49" s="116">
+      <c r="B49" s="108">
         <f>B43 + 2</f>
         <v>43500</v>
       </c>
-      <c r="C49" s="116" t="str">
-        <f t="shared" ref="C49:C57" si="7">IF(WEEKDAY(B49,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B49,1))</f>
+      <c r="C49" s="108" t="str">
+        <f t="shared" ref="C49:C57" si="8">IF(WEEKDAY(B49,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B49,1))</f>
         <v>Thứ 2</v>
       </c>
-      <c r="D49" s="117">
+      <c r="D49" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E49" s="118"/>
-      <c r="F49" s="119"/>
-      <c r="G49" s="119"/>
-      <c r="H49" s="119"/>
-      <c r="I49" s="120"/>
+      <c r="E49" s="110"/>
+      <c r="F49" s="111"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="112"/>
       <c r="J49" s="56"/>
       <c r="K49" s="56"/>
       <c r="L49" s="56"/>
@@ -6364,25 +6367,25 @@
       <c r="AA49" s="56"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A50" s="115" t="s">
+      <c r="A50" s="107" t="s">
         <v>374</v>
       </c>
-      <c r="B50" s="116">
+      <c r="B50" s="108">
         <f>B44 + 2</f>
         <v>43500</v>
       </c>
-      <c r="C50" s="116" t="str">
-        <f t="shared" si="7"/>
+      <c r="C50" s="108" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D50" s="117">
+      <c r="D50" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E50" s="118"/>
-      <c r="F50" s="119"/>
-      <c r="G50" s="119"/>
-      <c r="H50" s="119"/>
-      <c r="I50" s="120"/>
+      <c r="E50" s="110"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="112"/>
       <c r="J50" s="56"/>
       <c r="K50" s="56"/>
       <c r="L50" s="56"/>
@@ -6403,25 +6406,25 @@
       <c r="AA50" s="56"/>
     </row>
     <row r="51" spans="1:27" ht="15">
-      <c r="A51" s="133" t="s">
+      <c r="A51" s="125" t="s">
         <v>895</v>
       </c>
-      <c r="B51" s="130">
+      <c r="B51" s="122">
         <f>B45 + 2</f>
         <v>43500</v>
       </c>
-      <c r="C51" s="130" t="str">
-        <f t="shared" si="7"/>
+      <c r="C51" s="122" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D51" s="131">
+      <c r="D51" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E51" s="132"/>
-      <c r="F51" s="119"/>
-      <c r="G51" s="119"/>
-      <c r="H51" s="119"/>
-      <c r="I51" s="120"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="111"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="112"/>
       <c r="J51" s="56"/>
       <c r="K51" s="56"/>
       <c r="L51" s="56"/>
@@ -6442,25 +6445,25 @@
       <c r="AA51" s="56"/>
     </row>
     <row r="52" spans="1:27" ht="15">
-      <c r="A52" s="115" t="s">
+      <c r="A52" s="107" t="s">
         <v>367</v>
       </c>
-      <c r="B52" s="128">
+      <c r="B52" s="120">
         <f>B43+3</f>
         <v>43501</v>
       </c>
-      <c r="C52" s="116" t="str">
-        <f t="shared" si="7"/>
+      <c r="C52" s="108" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D52" s="117">
+      <c r="D52" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E52" s="118"/>
-      <c r="F52" s="119"/>
-      <c r="G52" s="119"/>
-      <c r="H52" s="119"/>
-      <c r="I52" s="120"/>
+      <c r="E52" s="110"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="111"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="112"/>
       <c r="J52" s="56"/>
       <c r="K52" s="56"/>
       <c r="L52" s="56"/>
@@ -6481,25 +6484,25 @@
       <c r="AA52" s="56"/>
     </row>
     <row r="53" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A53" s="115" t="s">
+      <c r="A53" s="107" t="s">
         <v>368</v>
       </c>
-      <c r="B53" s="128">
+      <c r="B53" s="120">
         <f>B44+3</f>
         <v>43501</v>
       </c>
-      <c r="C53" s="116" t="str">
-        <f t="shared" si="7"/>
+      <c r="C53" s="108" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D53" s="117">
+      <c r="D53" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E53" s="118"/>
-      <c r="F53" s="119"/>
-      <c r="G53" s="119"/>
-      <c r="H53" s="119"/>
-      <c r="I53" s="120"/>
+      <c r="E53" s="110"/>
+      <c r="F53" s="111"/>
+      <c r="G53" s="111"/>
+      <c r="H53" s="111"/>
+      <c r="I53" s="112"/>
       <c r="J53" s="56"/>
       <c r="K53" s="56"/>
       <c r="L53" s="56"/>
@@ -6520,25 +6523,25 @@
       <c r="AA53" s="56"/>
     </row>
     <row r="54" spans="1:27" ht="15">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="125" t="s">
         <v>898</v>
       </c>
-      <c r="B54" s="130">
+      <c r="B54" s="122">
         <f>B45+3</f>
         <v>43501</v>
       </c>
-      <c r="C54" s="130" t="str">
-        <f t="shared" si="7"/>
+      <c r="C54" s="122" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D54" s="131">
+      <c r="D54" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E54" s="132"/>
-      <c r="F54" s="119"/>
-      <c r="G54" s="119"/>
-      <c r="H54" s="119"/>
-      <c r="I54" s="120"/>
+      <c r="E54" s="124"/>
+      <c r="F54" s="111"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="112"/>
       <c r="J54" s="56"/>
       <c r="K54" s="56"/>
       <c r="L54" s="56"/>
@@ -6559,25 +6562,25 @@
       <c r="AA54" s="56"/>
     </row>
     <row r="55" spans="1:27" ht="15">
-      <c r="A55" s="115" t="s">
+      <c r="A55" s="107" t="s">
         <v>405</v>
       </c>
-      <c r="B55" s="116">
-        <f>B52 + 1</f>
+      <c r="B55" s="108">
+        <f t="shared" ref="B55:B60" si="9">B52 + 1</f>
         <v>43502</v>
       </c>
-      <c r="C55" s="116" t="str">
-        <f t="shared" si="7"/>
+      <c r="C55" s="108" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D55" s="117">
+      <c r="D55" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E55" s="118"/>
-      <c r="F55" s="119"/>
-      <c r="G55" s="119"/>
-      <c r="H55" s="119"/>
-      <c r="I55" s="120"/>
+      <c r="E55" s="110"/>
+      <c r="F55" s="111"/>
+      <c r="G55" s="111"/>
+      <c r="H55" s="111"/>
+      <c r="I55" s="112"/>
       <c r="J55" s="56"/>
       <c r="K55" s="56"/>
       <c r="L55" s="56"/>
@@ -6598,25 +6601,25 @@
       <c r="AA55" s="56"/>
     </row>
     <row r="56" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="107" t="s">
         <v>406</v>
       </c>
-      <c r="B56" s="116">
-        <f>B53 + 1</f>
+      <c r="B56" s="108">
+        <f t="shared" si="9"/>
         <v>43502</v>
       </c>
-      <c r="C56" s="116" t="str">
-        <f t="shared" si="7"/>
+      <c r="C56" s="108" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D56" s="117">
+      <c r="D56" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E56" s="118"/>
-      <c r="F56" s="119"/>
-      <c r="G56" s="119"/>
-      <c r="H56" s="119"/>
-      <c r="I56" s="120"/>
+      <c r="E56" s="110"/>
+      <c r="F56" s="111"/>
+      <c r="G56" s="111"/>
+      <c r="H56" s="111"/>
+      <c r="I56" s="112"/>
       <c r="J56" s="56"/>
       <c r="K56" s="56"/>
       <c r="L56" s="56"/>
@@ -6637,25 +6640,25 @@
       <c r="AA56" s="56"/>
     </row>
     <row r="57" spans="1:27" ht="15">
-      <c r="A57" s="133" t="s">
+      <c r="A57" s="125" t="s">
         <v>894</v>
       </c>
-      <c r="B57" s="130">
-        <f>B54 + 1</f>
+      <c r="B57" s="122">
+        <f t="shared" si="9"/>
         <v>43502</v>
       </c>
-      <c r="C57" s="130" t="str">
-        <f t="shared" si="7"/>
+      <c r="C57" s="122" t="str">
+        <f t="shared" si="8"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D57" s="131">
+      <c r="D57" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E57" s="132"/>
-      <c r="F57" s="119"/>
-      <c r="G57" s="119"/>
-      <c r="H57" s="119"/>
-      <c r="I57" s="120"/>
+      <c r="E57" s="124"/>
+      <c r="F57" s="111"/>
+      <c r="G57" s="111"/>
+      <c r="H57" s="111"/>
+      <c r="I57" s="112"/>
       <c r="J57" s="56"/>
       <c r="K57" s="56"/>
       <c r="L57" s="56"/>
@@ -6676,25 +6679,25 @@
       <c r="AA57" s="56"/>
     </row>
     <row r="58" spans="1:27" ht="15">
-      <c r="A58" s="115" t="s">
+      <c r="A58" s="107" t="s">
         <v>375</v>
       </c>
-      <c r="B58" s="116">
-        <f>B55 + 1</f>
+      <c r="B58" s="108">
+        <f t="shared" si="9"/>
         <v>43503</v>
       </c>
-      <c r="C58" s="116" t="str">
-        <f t="shared" ref="C58:C80" si="8">IF(WEEKDAY(B58,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B58,1))</f>
+      <c r="C58" s="108" t="str">
+        <f t="shared" ref="C58:C80" si="10">IF(WEEKDAY(B58,1)=1,"Chủ nhật","Thứ "&amp;WEEKDAY(B58,1))</f>
         <v>Thứ 5</v>
       </c>
-      <c r="D58" s="117">
+      <c r="D58" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E58" s="118"/>
-      <c r="F58" s="119"/>
-      <c r="G58" s="119"/>
-      <c r="H58" s="119"/>
-      <c r="I58" s="120"/>
+      <c r="E58" s="110"/>
+      <c r="F58" s="111"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="112"/>
       <c r="J58" s="56"/>
       <c r="K58" s="56"/>
       <c r="L58" s="56"/>
@@ -6715,25 +6718,25 @@
       <c r="AA58" s="56"/>
     </row>
     <row r="59" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A59" s="115" t="s">
+      <c r="A59" s="107" t="s">
         <v>376</v>
       </c>
-      <c r="B59" s="116">
-        <f>B56 + 1</f>
+      <c r="B59" s="108">
+        <f t="shared" si="9"/>
         <v>43503</v>
       </c>
-      <c r="C59" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C59" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D59" s="117">
+      <c r="D59" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E59" s="118"/>
-      <c r="F59" s="119"/>
-      <c r="G59" s="119"/>
-      <c r="H59" s="119"/>
-      <c r="I59" s="120"/>
+      <c r="E59" s="110"/>
+      <c r="F59" s="111"/>
+      <c r="G59" s="111"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="112"/>
       <c r="J59" s="56"/>
       <c r="K59" s="56"/>
       <c r="L59" s="56"/>
@@ -6754,25 +6757,25 @@
       <c r="AA59" s="56"/>
     </row>
     <row r="60" spans="1:27" ht="15">
-      <c r="A60" s="133" t="s">
+      <c r="A60" s="125" t="s">
         <v>895</v>
       </c>
-      <c r="B60" s="130">
-        <f>B57 + 1</f>
+      <c r="B60" s="122">
+        <f t="shared" si="9"/>
         <v>43503</v>
       </c>
-      <c r="C60" s="130" t="str">
-        <f t="shared" si="8"/>
+      <c r="C60" s="122" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D60" s="131">
+      <c r="D60" s="123">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E60" s="132"/>
-      <c r="F60" s="119"/>
-      <c r="G60" s="119"/>
-      <c r="H60" s="119"/>
-      <c r="I60" s="120"/>
+      <c r="E60" s="124"/>
+      <c r="F60" s="111"/>
+      <c r="G60" s="111"/>
+      <c r="H60" s="111"/>
+      <c r="I60" s="112"/>
       <c r="J60" s="56"/>
       <c r="K60" s="56"/>
       <c r="L60" s="56"/>
@@ -6793,25 +6796,25 @@
       <c r="AA60" s="56"/>
     </row>
     <row r="61" spans="1:27" ht="15">
-      <c r="A61" s="115" t="s">
+      <c r="A61" s="107" t="s">
         <v>377</v>
       </c>
-      <c r="B61" s="116">
+      <c r="B61" s="108">
         <f>B59 + 1</f>
         <v>43504</v>
       </c>
-      <c r="C61" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C61" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D61" s="117">
+      <c r="D61" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E61" s="118"/>
-      <c r="F61" s="119"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="120"/>
+      <c r="E61" s="110"/>
+      <c r="F61" s="111"/>
+      <c r="G61" s="111"/>
+      <c r="H61" s="111"/>
+      <c r="I61" s="112"/>
       <c r="J61" s="56"/>
       <c r="K61" s="56"/>
       <c r="L61" s="56"/>
@@ -6832,27 +6835,27 @@
       <c r="AA61" s="56"/>
     </row>
     <row r="62" spans="1:27" ht="15">
-      <c r="A62" s="115" t="s">
+      <c r="A62" s="107" t="s">
         <v>407</v>
       </c>
-      <c r="B62" s="116">
+      <c r="B62" s="108">
         <f>B59 + 1</f>
         <v>43504</v>
       </c>
-      <c r="C62" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C62" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D62" s="117">
+      <c r="D62" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E62" s="118"/>
-      <c r="F62" s="119"/>
-      <c r="G62" s="119"/>
-      <c r="H62" s="119"/>
-      <c r="I62" s="120"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="111"/>
+      <c r="G62" s="111"/>
+      <c r="H62" s="111"/>
+      <c r="I62" s="112"/>
       <c r="J62" s="56"/>
-      <c r="K62" s="101"/>
+      <c r="K62" s="93"/>
       <c r="L62" s="56"/>
       <c r="M62" s="56"/>
       <c r="N62" s="56"/>
@@ -6871,25 +6874,25 @@
       <c r="AA62" s="56"/>
     </row>
     <row r="63" spans="1:27" ht="15">
-      <c r="A63" s="115" t="s">
+      <c r="A63" s="107" t="s">
         <v>408</v>
       </c>
-      <c r="B63" s="116">
+      <c r="B63" s="108">
         <f>B59 +1</f>
         <v>43504</v>
       </c>
-      <c r="C63" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C63" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D63" s="117">
+      <c r="D63" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E63" s="118"/>
-      <c r="F63" s="119"/>
-      <c r="G63" s="119"/>
-      <c r="H63" s="119"/>
-      <c r="I63" s="120"/>
+      <c r="E63" s="110"/>
+      <c r="F63" s="111"/>
+      <c r="G63" s="111"/>
+      <c r="H63" s="111"/>
+      <c r="I63" s="112"/>
       <c r="J63" s="56"/>
       <c r="K63" s="56"/>
       <c r="L63" s="56"/>
@@ -6910,27 +6913,27 @@
       <c r="AA63" s="56"/>
     </row>
     <row r="64" spans="1:27" ht="15">
-      <c r="A64" s="115" t="s">
+      <c r="A64" s="107" t="s">
         <v>378</v>
       </c>
-      <c r="B64" s="116">
+      <c r="B64" s="108">
         <f>B59 +2</f>
         <v>43505</v>
       </c>
-      <c r="C64" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C64" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D64" s="117">
+      <c r="D64" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E64" s="118" t="s">
+      <c r="E64" s="110" t="s">
         <v>392</v>
       </c>
-      <c r="F64" s="119"/>
-      <c r="G64" s="119"/>
-      <c r="H64" s="119"/>
-      <c r="I64" s="120"/>
+      <c r="F64" s="111"/>
+      <c r="G64" s="111"/>
+      <c r="H64" s="111"/>
+      <c r="I64" s="112"/>
       <c r="J64" s="56"/>
       <c r="K64" s="56"/>
       <c r="L64" s="56"/>
@@ -6951,25 +6954,25 @@
       <c r="AA64" s="56"/>
     </row>
     <row r="65" spans="1:27" ht="15">
-      <c r="A65" s="115" t="s">
+      <c r="A65" s="107" t="s">
         <v>379</v>
       </c>
-      <c r="B65" s="116">
+      <c r="B65" s="108">
         <f>B61 + 1</f>
         <v>43505</v>
       </c>
-      <c r="C65" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C65" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D65" s="117">
+      <c r="D65" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E65" s="118"/>
-      <c r="F65" s="119"/>
-      <c r="G65" s="119"/>
-      <c r="H65" s="119"/>
-      <c r="I65" s="120"/>
+      <c r="E65" s="110"/>
+      <c r="F65" s="111"/>
+      <c r="G65" s="111"/>
+      <c r="H65" s="111"/>
+      <c r="I65" s="112"/>
       <c r="J65" s="56"/>
       <c r="K65" s="56"/>
       <c r="L65" s="56"/>
@@ -6990,25 +6993,25 @@
       <c r="AA65" s="56"/>
     </row>
     <row r="66" spans="1:27" ht="15">
-      <c r="A66" s="115" t="s">
+      <c r="A66" s="107" t="s">
         <v>380</v>
       </c>
-      <c r="B66" s="116">
+      <c r="B66" s="108">
         <f>B61 +1</f>
         <v>43505</v>
       </c>
-      <c r="C66" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C66" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D66" s="117">
+      <c r="D66" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E66" s="118"/>
-      <c r="F66" s="119"/>
-      <c r="G66" s="119"/>
-      <c r="H66" s="119"/>
-      <c r="I66" s="120"/>
+      <c r="E66" s="110"/>
+      <c r="F66" s="111"/>
+      <c r="G66" s="111"/>
+      <c r="H66" s="111"/>
+      <c r="I66" s="112"/>
       <c r="J66" s="56"/>
       <c r="K66" s="56"/>
       <c r="L66" s="56"/>
@@ -7029,25 +7032,25 @@
       <c r="AA66" s="56"/>
     </row>
     <row r="67" spans="1:27" ht="15">
-      <c r="A67" s="115" t="s">
+      <c r="A67" s="107" t="s">
         <v>409</v>
       </c>
-      <c r="B67" s="116">
-        <f t="shared" ref="B67:B75" si="9">B63 + 2</f>
+      <c r="B67" s="108">
+        <f t="shared" ref="B67:B73" si="11">B63 + 2</f>
         <v>43506</v>
       </c>
-      <c r="C67" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C67" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D67" s="117">
+      <c r="D67" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E67" s="118"/>
-      <c r="F67" s="119"/>
-      <c r="G67" s="119"/>
-      <c r="H67" s="119"/>
-      <c r="I67" s="120"/>
+      <c r="E67" s="110"/>
+      <c r="F67" s="111"/>
+      <c r="G67" s="111"/>
+      <c r="H67" s="111"/>
+      <c r="I67" s="112"/>
       <c r="J67" s="56"/>
       <c r="K67" s="56"/>
       <c r="L67" s="56"/>
@@ -7068,27 +7071,27 @@
       <c r="AA67" s="56"/>
     </row>
     <row r="68" spans="1:27" ht="15">
-      <c r="A68" s="115" t="s">
+      <c r="A68" s="107" t="s">
         <v>354</v>
       </c>
-      <c r="B68" s="116">
+      <c r="B68" s="108">
         <f>B64 + 1</f>
         <v>43506</v>
       </c>
-      <c r="C68" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C68" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D68" s="117">
+      <c r="D68" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E68" s="118" t="s">
+      <c r="E68" s="110" t="s">
         <v>392</v>
       </c>
-      <c r="F68" s="119"/>
-      <c r="G68" s="119"/>
-      <c r="H68" s="119"/>
-      <c r="I68" s="120"/>
+      <c r="F68" s="111"/>
+      <c r="G68" s="111"/>
+      <c r="H68" s="111"/>
+      <c r="I68" s="112"/>
       <c r="J68" s="56"/>
       <c r="K68" s="56"/>
       <c r="L68" s="56"/>
@@ -7109,25 +7112,25 @@
       <c r="AA68" s="56"/>
     </row>
     <row r="69" spans="1:27" ht="15">
-      <c r="A69" s="115" t="s">
+      <c r="A69" s="107" t="s">
         <v>381</v>
       </c>
-      <c r="B69" s="116">
+      <c r="B69" s="108">
         <f>B65 + 1</f>
         <v>43506</v>
       </c>
-      <c r="C69" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C69" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D69" s="117">
+      <c r="D69" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E69" s="118"/>
-      <c r="F69" s="119"/>
-      <c r="G69" s="119"/>
-      <c r="H69" s="119"/>
-      <c r="I69" s="120"/>
+      <c r="E69" s="110"/>
+      <c r="F69" s="111"/>
+      <c r="G69" s="111"/>
+      <c r="H69" s="111"/>
+      <c r="I69" s="112"/>
       <c r="J69" s="56"/>
       <c r="K69" s="56"/>
       <c r="L69" s="56"/>
@@ -7148,25 +7151,25 @@
       <c r="AA69" s="56"/>
     </row>
     <row r="70" spans="1:27" ht="15">
-      <c r="A70" s="115" t="s">
+      <c r="A70" s="107" t="s">
         <v>382</v>
       </c>
-      <c r="B70" s="116">
-        <f t="shared" si="9"/>
+      <c r="B70" s="108">
+        <f t="shared" si="11"/>
         <v>43507</v>
       </c>
-      <c r="C70" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C70" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D70" s="117">
+      <c r="D70" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E70" s="118"/>
-      <c r="F70" s="119"/>
-      <c r="G70" s="119"/>
-      <c r="H70" s="119"/>
-      <c r="I70" s="120"/>
+      <c r="E70" s="110"/>
+      <c r="F70" s="111"/>
+      <c r="G70" s="111"/>
+      <c r="H70" s="111"/>
+      <c r="I70" s="112"/>
       <c r="J70" s="56"/>
       <c r="K70" s="56"/>
       <c r="L70" s="56"/>
@@ -7187,25 +7190,25 @@
       <c r="AA70" s="56"/>
     </row>
     <row r="71" spans="1:27" ht="15">
-      <c r="A71" s="115" t="s">
+      <c r="A71" s="107" t="s">
         <v>383</v>
       </c>
-      <c r="B71" s="116">
+      <c r="B71" s="108">
         <f>B67 + 1</f>
         <v>43507</v>
       </c>
-      <c r="C71" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C71" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D71" s="117">
+      <c r="D71" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E71" s="118"/>
-      <c r="F71" s="119"/>
-      <c r="G71" s="119"/>
-      <c r="H71" s="119"/>
-      <c r="I71" s="120"/>
+      <c r="E71" s="110"/>
+      <c r="F71" s="111"/>
+      <c r="G71" s="111"/>
+      <c r="H71" s="111"/>
+      <c r="I71" s="112"/>
       <c r="J71" s="56"/>
       <c r="K71" s="56"/>
       <c r="L71" s="56"/>
@@ -7226,25 +7229,25 @@
       <c r="AA71" s="56"/>
     </row>
     <row r="72" spans="1:27" ht="15">
-      <c r="A72" s="115" t="s">
+      <c r="A72" s="107" t="s">
         <v>410</v>
       </c>
-      <c r="B72" s="116">
+      <c r="B72" s="108">
         <f>B68 + 1</f>
         <v>43507</v>
       </c>
-      <c r="C72" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C72" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 2</v>
       </c>
-      <c r="D72" s="117">
+      <c r="D72" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E72" s="118"/>
-      <c r="F72" s="119"/>
-      <c r="G72" s="119"/>
-      <c r="H72" s="119"/>
-      <c r="I72" s="120"/>
+      <c r="E72" s="110"/>
+      <c r="F72" s="111"/>
+      <c r="G72" s="111"/>
+      <c r="H72" s="111"/>
+      <c r="I72" s="112"/>
       <c r="J72" s="56"/>
       <c r="K72" s="56"/>
       <c r="L72" s="56"/>
@@ -7265,25 +7268,25 @@
       <c r="AA72" s="56"/>
     </row>
     <row r="73" spans="1:27" ht="15">
-      <c r="A73" s="115" t="s">
+      <c r="A73" s="107" t="s">
         <v>411</v>
       </c>
-      <c r="B73" s="116">
-        <f t="shared" si="9"/>
+      <c r="B73" s="108">
+        <f t="shared" si="11"/>
         <v>43508</v>
       </c>
-      <c r="C73" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C73" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D73" s="117">
+      <c r="D73" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E73" s="118"/>
-      <c r="F73" s="119"/>
-      <c r="G73" s="119"/>
-      <c r="H73" s="119"/>
-      <c r="I73" s="120"/>
+      <c r="E73" s="110"/>
+      <c r="F73" s="111"/>
+      <c r="G73" s="111"/>
+      <c r="H73" s="111"/>
+      <c r="I73" s="112"/>
       <c r="J73" s="56"/>
       <c r="K73" s="56"/>
       <c r="L73" s="56"/>
@@ -7304,25 +7307,25 @@
       <c r="AA73" s="56"/>
     </row>
     <row r="74" spans="1:27" ht="15">
-      <c r="A74" s="115" t="s">
+      <c r="A74" s="107" t="s">
         <v>384</v>
       </c>
-      <c r="B74" s="116">
+      <c r="B74" s="108">
         <f>B70 + 1</f>
         <v>43508</v>
       </c>
-      <c r="C74" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C74" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D74" s="117">
+      <c r="D74" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E74" s="118"/>
-      <c r="F74" s="119"/>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119"/>
-      <c r="I74" s="120"/>
+      <c r="E74" s="110"/>
+      <c r="F74" s="111"/>
+      <c r="G74" s="111"/>
+      <c r="H74" s="111"/>
+      <c r="I74" s="112"/>
       <c r="J74" s="56"/>
       <c r="K74" s="56"/>
       <c r="L74" s="56"/>
@@ -7343,25 +7346,25 @@
       <c r="AA74" s="56"/>
     </row>
     <row r="75" spans="1:27" ht="15">
-      <c r="A75" s="115" t="s">
+      <c r="A75" s="107" t="s">
         <v>385</v>
       </c>
-      <c r="B75" s="116">
+      <c r="B75" s="108">
         <f>B71 + 1</f>
         <v>43508</v>
       </c>
-      <c r="C75" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C75" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 3</v>
       </c>
-      <c r="D75" s="117">
+      <c r="D75" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E75" s="118"/>
-      <c r="F75" s="119"/>
-      <c r="G75" s="119"/>
-      <c r="H75" s="119"/>
-      <c r="I75" s="120"/>
+      <c r="E75" s="110"/>
+      <c r="F75" s="111"/>
+      <c r="G75" s="111"/>
+      <c r="H75" s="111"/>
+      <c r="I75" s="112"/>
       <c r="J75" s="56"/>
       <c r="K75" s="56"/>
       <c r="L75" s="56"/>
@@ -7382,25 +7385,25 @@
       <c r="AA75" s="56"/>
     </row>
     <row r="76" spans="1:27" ht="15">
-      <c r="A76" s="115" t="s">
+      <c r="A76" s="107" t="s">
         <v>386</v>
       </c>
-      <c r="B76" s="116">
+      <c r="B76" s="108">
         <f>B72 + 2</f>
         <v>43509</v>
       </c>
-      <c r="C76" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C76" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 4</v>
       </c>
-      <c r="D76" s="117">
+      <c r="D76" s="109">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E76" s="118"/>
-      <c r="F76" s="119"/>
-      <c r="G76" s="119"/>
-      <c r="H76" s="119"/>
-      <c r="I76" s="120"/>
+      <c r="E76" s="110"/>
+      <c r="F76" s="111"/>
+      <c r="G76" s="111"/>
+      <c r="H76" s="111"/>
+      <c r="I76" s="112"/>
       <c r="J76" s="56"/>
       <c r="K76" s="56"/>
       <c r="L76" s="56"/>
@@ -7421,25 +7424,25 @@
       <c r="AA76" s="56"/>
     </row>
     <row r="77" spans="1:27" ht="15">
-      <c r="A77" s="115" t="s">
+      <c r="A77" s="107" t="s">
         <v>387</v>
       </c>
-      <c r="B77" s="116">
+      <c r="B77" s="108">
         <f>B73 +2</f>
         <v>43510</v>
       </c>
-      <c r="C77" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C77" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 5</v>
       </c>
-      <c r="D77" s="117">
+      <c r="D77" s="109">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E77" s="118"/>
-      <c r="F77" s="119"/>
-      <c r="G77" s="119"/>
-      <c r="H77" s="119"/>
-      <c r="I77" s="120"/>
+      <c r="E77" s="110"/>
+      <c r="F77" s="111"/>
+      <c r="G77" s="111"/>
+      <c r="H77" s="111"/>
+      <c r="I77" s="112"/>
       <c r="J77" s="55"/>
       <c r="K77" s="56"/>
       <c r="L77" s="56"/>
@@ -7460,25 +7463,25 @@
       <c r="AA77" s="56"/>
     </row>
     <row r="78" spans="1:27" ht="15">
-      <c r="A78" s="115" t="s">
+      <c r="A78" s="107" t="s">
         <v>388</v>
       </c>
-      <c r="B78" s="116">
+      <c r="B78" s="108">
         <f>B73 + 3</f>
         <v>43511</v>
       </c>
-      <c r="C78" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C78" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 6</v>
       </c>
-      <c r="D78" s="117">
+      <c r="D78" s="109">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E78" s="118"/>
-      <c r="F78" s="119"/>
-      <c r="G78" s="119"/>
-      <c r="H78" s="119"/>
-      <c r="I78" s="120"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="111"/>
+      <c r="G78" s="111"/>
+      <c r="H78" s="111"/>
+      <c r="I78" s="112"/>
       <c r="J78" s="55"/>
       <c r="K78" s="56"/>
       <c r="L78" s="56"/>
@@ -7499,25 +7502,25 @@
       <c r="AA78" s="56"/>
     </row>
     <row r="79" spans="1:27" ht="15">
-      <c r="A79" s="115" t="s">
+      <c r="A79" s="107" t="s">
         <v>389</v>
       </c>
-      <c r="B79" s="116">
+      <c r="B79" s="108">
         <f>B75 + 4</f>
         <v>43512</v>
       </c>
-      <c r="C79" s="116" t="str">
-        <f t="shared" si="8"/>
+      <c r="C79" s="108" t="str">
+        <f t="shared" si="10"/>
         <v>Thứ 7</v>
       </c>
-      <c r="D79" s="117">
+      <c r="D79" s="109">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E79" s="118"/>
-      <c r="F79" s="119"/>
-      <c r="G79" s="119"/>
-      <c r="H79" s="119"/>
-      <c r="I79" s="120"/>
+      <c r="E79" s="110"/>
+      <c r="F79" s="111"/>
+      <c r="G79" s="111"/>
+      <c r="H79" s="111"/>
+      <c r="I79" s="112"/>
       <c r="J79" s="55"/>
       <c r="K79" s="56"/>
       <c r="L79" s="56"/>
@@ -7538,27 +7541,27 @@
       <c r="AA79" s="56"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" thickBot="1">
-      <c r="A80" s="122" t="s">
+      <c r="A80" s="114" t="s">
         <v>390</v>
       </c>
-      <c r="B80" s="123">
+      <c r="B80" s="115">
         <f>B76 + 4</f>
         <v>43513</v>
       </c>
-      <c r="C80" s="123" t="str">
-        <f t="shared" si="8"/>
+      <c r="C80" s="115" t="str">
+        <f t="shared" si="10"/>
         <v>Chủ nhật</v>
       </c>
-      <c r="D80" s="124">
+      <c r="D80" s="116">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E80" s="125"/>
-      <c r="F80" s="126" t="s">
+      <c r="E80" s="117"/>
+      <c r="F80" s="118" t="s">
         <v>788</v>
       </c>
-      <c r="G80" s="126"/>
-      <c r="H80" s="126"/>
-      <c r="I80" s="127"/>
+      <c r="G80" s="118"/>
+      <c r="H80" s="118"/>
+      <c r="I80" s="119"/>
       <c r="J80" s="56"/>
       <c r="K80" s="56"/>
       <c r="L80" s="56"/>
@@ -34319,8 +34322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AD6CE4-A652-4BA6-AF5B-7B55F9607709}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34495,14 +34498,18 @@
       <c r="E13" s="75"/>
       <c r="F13" s="76"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="45">
       <c r="A14" s="72">
         <v>13</v>
       </c>
       <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
+      <c r="C14" s="72" t="s">
+        <v>4</v>
+      </c>
       <c r="D14" s="71"/>
-      <c r="E14" s="75"/>
+      <c r="E14" s="75" t="s">
+        <v>899</v>
+      </c>
       <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:8">
@@ -45189,152 +45196,152 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="128" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="128" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="128" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="130"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="128" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="128" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="97"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="130"/>
     </row>
     <row r="9" spans="1:11" ht="99.75" customHeight="1" thickBot="1">
       <c r="A9" s="10"/>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="131" t="s">
         <v>220</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="100"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -45365,231 +45372,225 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="128" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="128" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="130"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="128" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="128" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="128" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
     </row>
     <row r="8" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="128" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="97"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="130"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="128" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="97"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="130"/>
     </row>
     <row r="10" spans="1:11" ht="60" customHeight="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="128" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="97"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="130"/>
     </row>
     <row r="11" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="97"/>
+      <c r="C11" s="129"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="130"/>
     </row>
     <row r="12" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A12" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="128" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="97"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="130"/>
     </row>
     <row r="13" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="128" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="97"/>
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -45597,6 +45598,12 @@
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45778,120 +45785,120 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="128" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="128" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="128" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="130"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="128" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="128" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -45923,120 +45930,120 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="128" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="130"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="128" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -46068,135 +46075,135 @@
       <c r="A1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="128" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="128" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
     </row>
     <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="128" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="130"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="128" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="97"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="130"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="128" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="97"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="130"/>
     </row>
     <row r="8" spans="1:11" ht="150.75" customHeight="1" thickBot="1">
       <c r="A8" s="10"/>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="100"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
co len co len
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
+++ b/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42BC3F1-CB89-4222-86D9-7FD9E20352B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FBE902-368B-429C-9140-91F23125A7D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="600" firstSheet="10" activeTab="15" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="906">
   <si>
     <t>No</t>
   </si>
@@ -2969,6 +2969,24 @@
   </si>
   <si>
     <t>Milestones significant (đánh dấu) events within the project schedule. Chúng k phải là work activities. They have no duration</t>
+  </si>
+  <si>
+    <t>first cần ngồi cùng với team để determine the impact on the project và evaluate alternative solutions. Khi đã come up with recommendations bạn có thể present them to management and customer</t>
+  </si>
+  <si>
+    <t>PM có trách nhiệm manage the project scope completion within budget including the contigency reserves allocates for this identified risk</t>
+  </si>
+  <si>
+    <t>PM cần phải obtain change control board approval to affect the change</t>
+  </si>
+  <si>
+    <t>nếu activity nằm trên critical path thì cần phải lựa chọn quyết định change hay không? Và cần phải có CCB approval. cần phải evaluate và identify options có sử dụng float. Nếu nó không nằm trên critical path thì cần tìm possibly look for time from another activity</t>
+  </si>
+  <si>
+    <t>có problem đầu tiên là phải evaluate. Việc xác định cost variance đầu tiên có thể đưa ra solution các activities can be done parallel</t>
+  </si>
+  <si>
+    <t>Network diagram thể hiện rõ ràng các interdependencies hơn bar chart</t>
   </si>
 </sst>
 </file>
@@ -34322,8 +34340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AD6CE4-A652-4BA6-AF5B-7B55F9607709}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34522,44 +34540,52 @@
       <c r="E15" s="75"/>
       <c r="F15" s="76"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="75">
       <c r="A16" s="72">
         <v>15</v>
       </c>
       <c r="B16" s="72"/>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
-      <c r="E16" s="75"/>
+      <c r="E16" s="75" t="s">
+        <v>900</v>
+      </c>
       <c r="F16" s="76"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="60">
       <c r="A17" s="72">
         <v>16</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" s="72"/>
       <c r="D17" s="72"/>
-      <c r="E17" s="75"/>
+      <c r="E17" s="75" t="s">
+        <v>901</v>
+      </c>
       <c r="F17" s="76"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="72">
         <v>17</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="72"/>
       <c r="D18" s="72"/>
-      <c r="E18" s="75"/>
+      <c r="E18" s="75" t="s">
+        <v>902</v>
+      </c>
       <c r="F18" s="76"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="90">
       <c r="A19" s="72">
         <v>18</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>
       <c r="D19" s="72"/>
-      <c r="E19" s="75"/>
+      <c r="E19" s="75" t="s">
+        <v>903</v>
+      </c>
       <c r="F19" s="76"/>
     </row>
     <row r="20" spans="1:6">
@@ -34572,24 +34598,28 @@
       <c r="E20" s="75"/>
       <c r="F20" s="76"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="45">
       <c r="A21" s="72">
         <v>20</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="72"/>
       <c r="D21" s="72"/>
-      <c r="E21" s="75"/>
+      <c r="E21" s="75" t="s">
+        <v>904</v>
+      </c>
       <c r="F21" s="76"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="72">
         <v>21</v>
       </c>
       <c r="B22" s="72"/>
       <c r="C22" s="72"/>
       <c r="D22" s="72"/>
-      <c r="E22" s="75"/>
+      <c r="E22" s="75" t="s">
+        <v>905</v>
+      </c>
       <c r="F22" s="76"/>
     </row>
     <row r="23" spans="1:6">
@@ -45591,6 +45621,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -45598,12 +45634,6 @@
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tap trung tap trung tap trung
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
+++ b/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CFECC8-CAE2-490F-ACBF-79819826F66A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08FD30E-C450-43C8-8DBA-0D314711D89A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="12" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
   <sheets>
     <sheet name="study plan" sheetId="22" r:id="rId1"/>
@@ -43,27 +43,28 @@
     <sheet name="Closing 1" sheetId="20" r:id="rId28"/>
     <sheet name="Initiating 2" sheetId="34" r:id="rId29"/>
     <sheet name="Initiating 3" sheetId="42" r:id="rId30"/>
-    <sheet name="Initiating 4" sheetId="54" r:id="rId31"/>
-    <sheet name="Initiating 1" sheetId="7" r:id="rId32"/>
-    <sheet name="Scope" sheetId="10" r:id="rId33"/>
-    <sheet name="Planning5" sheetId="3" r:id="rId34"/>
-    <sheet name="Planning1" sheetId="11" r:id="rId35"/>
-    <sheet name="Planning3" sheetId="16" r:id="rId36"/>
-    <sheet name="Executing1" sheetId="15" r:id="rId37"/>
-    <sheet name="Executing 4" sheetId="53" r:id="rId38"/>
-    <sheet name="Executing 3" sheetId="36" r:id="rId39"/>
-    <sheet name="Executing 8" sheetId="44" r:id="rId40"/>
-    <sheet name="Executing 2" sheetId="17" r:id="rId41"/>
-    <sheet name="Domain-Initiating" sheetId="18" r:id="rId42"/>
-    <sheet name="Domain-Planning" sheetId="12" r:id="rId43"/>
-    <sheet name="Domain-Executing" sheetId="13" r:id="rId44"/>
-    <sheet name="Domain-Monitoring &amp; Controlling" sheetId="14" r:id="rId45"/>
-    <sheet name="Domain-Closing" sheetId="19" r:id="rId46"/>
-    <sheet name="Executing" sheetId="4" r:id="rId47"/>
-    <sheet name="Monitoring" sheetId="5" r:id="rId48"/>
-    <sheet name="Closing" sheetId="6" r:id="rId49"/>
-    <sheet name="Mock" sheetId="8" r:id="rId50"/>
-    <sheet name="Full Test 4" sheetId="9" r:id="rId51"/>
+    <sheet name="Initiating 5" sheetId="56" r:id="rId31"/>
+    <sheet name="Initiating 4" sheetId="54" r:id="rId32"/>
+    <sheet name="Initiating 1" sheetId="7" r:id="rId33"/>
+    <sheet name="Scope" sheetId="10" r:id="rId34"/>
+    <sheet name="Planning5" sheetId="3" r:id="rId35"/>
+    <sheet name="Planning1" sheetId="11" r:id="rId36"/>
+    <sheet name="Planning3" sheetId="16" r:id="rId37"/>
+    <sheet name="Executing1" sheetId="15" r:id="rId38"/>
+    <sheet name="Executing 4" sheetId="53" r:id="rId39"/>
+    <sheet name="Executing 3" sheetId="36" r:id="rId40"/>
+    <sheet name="Executing 8" sheetId="44" r:id="rId41"/>
+    <sheet name="Executing 2" sheetId="17" r:id="rId42"/>
+    <sheet name="Domain-Initiating" sheetId="18" r:id="rId43"/>
+    <sheet name="Domain-Planning" sheetId="12" r:id="rId44"/>
+    <sheet name="Domain-Executing" sheetId="13" r:id="rId45"/>
+    <sheet name="Domain-Monitoring &amp; Controlling" sheetId="14" r:id="rId46"/>
+    <sheet name="Domain-Closing" sheetId="19" r:id="rId47"/>
+    <sheet name="Executing" sheetId="4" r:id="rId48"/>
+    <sheet name="Monitoring" sheetId="5" r:id="rId49"/>
+    <sheet name="Closing" sheetId="6" r:id="rId50"/>
+    <sheet name="Mock" sheetId="8" r:id="rId51"/>
+    <sheet name="Full Test 4" sheetId="9" r:id="rId52"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="1067">
   <si>
     <t>No</t>
   </si>
@@ -3432,6 +3433,49 @@
   </si>
   <si>
     <t>discount cash flow: dòng tiền chiết khấu. Pareto sử dụng để xác định most significant factors out of many( xác định các yếu tố quan trong nhất trong nhiều yếu tố), earned value management là monitor and controlling cost đang diễn ra (on going).monte carlo là technique để analysis risk</t>
+  </si>
+  <si>
+    <t>sponsor có thể help plan some of the activities nhưng nó không phải là their duty. Some project constraints từ sponsor nhưng nên được xem là necessary. The project management plan đc tạo ra với team và approved bơi sponsor and other management. Objective started trong project charter nên sponsor sẽ helping to prevent unnecessary change to project objectives</t>
+  </si>
+  <si>
+    <t>Note: project team knowledge ( recollection - hồi ức) đáng tin cậy hơn là document - trong văn cảnh này thì phải dựa vào project team knowledge</t>
+  </si>
+  <si>
+    <t>matrix organization là involves people nên communication là more complex</t>
+  </si>
+  <si>
+    <t>Do trong matrix organization team member phải report to PM và functional manager nên họ sẽ worried về vấn đề evaluated như là khoản fringe benefits</t>
+  </si>
+  <si>
+    <t>Nên đọc câu trả lời trc</t>
+  </si>
+  <si>
+    <t>Keyword: phải attempt to gain a complete product desciption before the project is initiated là chính xác</t>
+  </si>
+  <si>
+    <t>the project management process always includes the work of initiating, planning, executing, monitor &amp; controlling,  closing a project. This method là giống nhau cho tất cả các dự án</t>
+  </si>
+  <si>
+    <t>Stakeholders can be identified throughout the project</t>
+  </si>
+  <si>
+    <t>Ensuring continuing understanding of the work, removing roadblocks, and reviewing bids in order to select sellers all occur in project executing. Ensuring the product scope is as final as possible is done in project initiating.</t>
+  </si>
+  <si>
+    <t>create a detailed description of the project deliverable nằm trong planning, 1 phần của creating project scope statement.
+Root cause of problem in during monitoring and controlling, not initiating. Ensure all project management processes are complete in closing project</t>
+  </si>
+  <si>
+    <t>evaluate the effectiveness of risk responses and recommend changes and defect repair nằm trong monitoring and controlling. Update corporate processes and procedures based on lessons learned nằm trong closing project</t>
+  </si>
+  <si>
+    <t>Đặc điểm của project management processes là iterative (lặp đi lặp lại)</t>
+  </si>
+  <si>
+    <t>progressive elaboration means: project process are iterated as more information uncovered throughout project life cycle</t>
+  </si>
+  <si>
+    <t>Chưa làm</t>
   </si>
 </sst>
 </file>
@@ -4770,8 +4814,8 @@
   </sheetPr>
   <dimension ref="A1:AA1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -5648,7 +5692,9 @@
       <c r="H21" s="60" t="s">
         <v>475</v>
       </c>
-      <c r="I21" s="60"/>
+      <c r="I21" s="60" t="s">
+        <v>546</v>
+      </c>
       <c r="J21" s="56"/>
       <c r="K21" s="56"/>
       <c r="L21" s="56"/>
@@ -6229,10 +6275,10 @@
       <c r="D35" s="109">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E35" s="110"/>
-      <c r="F35" s="111" t="s">
-        <v>785</v>
-      </c>
+      <c r="E35" s="110" t="s">
+        <v>392</v>
+      </c>
+      <c r="F35" s="111"/>
       <c r="G35" s="111"/>
       <c r="H35" s="111" t="s">
         <v>484</v>
@@ -6299,7 +6345,7 @@
       <c r="AA36" s="56"/>
     </row>
     <row r="37" spans="1:27" ht="15">
-      <c r="A37" s="107" t="s">
+      <c r="A37" s="126" t="s">
         <v>363</v>
       </c>
       <c r="B37" s="108">
@@ -6313,10 +6359,10 @@
       <c r="D37" s="109">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E37" s="110"/>
-      <c r="F37" s="111" t="s">
-        <v>785</v>
-      </c>
+      <c r="E37" s="110" t="s">
+        <v>392</v>
+      </c>
+      <c r="F37" s="111"/>
       <c r="G37" s="111"/>
       <c r="H37" s="111" t="s">
         <v>485</v>
@@ -6699,7 +6745,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E46" s="110"/>
-      <c r="F46" s="111"/>
+      <c r="F46" s="111" t="s">
+        <v>546</v>
+      </c>
       <c r="G46" s="111"/>
       <c r="H46" s="111" t="s">
         <v>491</v>
@@ -6742,7 +6790,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E47" s="110"/>
-      <c r="F47" s="111"/>
+      <c r="F47" s="111" t="s">
+        <v>574</v>
+      </c>
       <c r="G47" s="111"/>
       <c r="H47" s="111"/>
       <c r="I47" s="112"/>
@@ -6820,7 +6870,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E49" s="110"/>
-      <c r="F49" s="111"/>
+      <c r="F49" s="111" t="s">
+        <v>574</v>
+      </c>
       <c r="G49" s="111"/>
       <c r="H49" s="111"/>
       <c r="I49" s="112"/>
@@ -6859,7 +6911,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E50" s="110"/>
-      <c r="F50" s="111"/>
+      <c r="F50" s="111" t="s">
+        <v>574</v>
+      </c>
       <c r="G50" s="111"/>
       <c r="H50" s="111"/>
       <c r="I50" s="112"/>
@@ -6937,7 +6991,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E52" s="110"/>
-      <c r="F52" s="111"/>
+      <c r="F52" s="111" t="s">
+        <v>1066</v>
+      </c>
       <c r="G52" s="111"/>
       <c r="H52" s="111"/>
       <c r="I52" s="112"/>
@@ -6976,7 +7032,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E53" s="110"/>
-      <c r="F53" s="111"/>
+      <c r="F53" s="111" t="s">
+        <v>546</v>
+      </c>
       <c r="G53" s="111"/>
       <c r="H53" s="111"/>
       <c r="I53" s="112"/>
@@ -7054,7 +7112,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E55" s="110"/>
-      <c r="F55" s="111"/>
+      <c r="F55" s="111" t="s">
+        <v>574</v>
+      </c>
       <c r="G55" s="111"/>
       <c r="H55" s="111"/>
       <c r="I55" s="112"/>
@@ -7093,7 +7153,9 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E56" s="110"/>
-      <c r="F56" s="111"/>
+      <c r="F56" s="111" t="s">
+        <v>574</v>
+      </c>
       <c r="G56" s="111"/>
       <c r="H56" s="111"/>
       <c r="I56" s="112"/>
@@ -31540,6 +31602,7 @@
     <hyperlink ref="A31" location="'Executing 4'!A1" display="Executing 4 - 50" xr:uid="{38A9238E-A836-47EC-AAAA-7B65A31FB899}"/>
     <hyperlink ref="A32" location="'Initiating 4'!A1" display="Initiating 4 - 25" xr:uid="{6A84B5A2-AB81-4C3F-AB87-82F3A6679E3B}"/>
     <hyperlink ref="A35" location="'Mock Exam 4'!A1" display="Mock Exam 4" xr:uid="{254B4A8E-2837-4015-8874-5E349804BC30}"/>
+    <hyperlink ref="A37" location="'Initiating 5'!A1" display="Initiating 5 - 25" xr:uid="{17043A15-97D7-4E15-8A7E-ECB8F04BD0E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -33015,7 +33078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD440D0-468F-462B-9532-3FA36BB45DDC}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D44" activeCellId="1" sqref="E46 D44"/>
     </sheetView>
   </sheetViews>
@@ -41708,11 +41771,355 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E7F72C-8763-4FD0-9393-7A7E1BDC492D}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="71"/>
+    <col min="2" max="2" width="65.85546875" style="71" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="71" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" style="71" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="71" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="71"/>
+    <col min="7" max="7" width="29.7109375" style="71" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="71"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="72">
+        <v>1</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="72">
+        <v>2</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="72">
+        <v>3</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
+    </row>
+    <row r="5" spans="1:6" ht="150">
+      <c r="A5" s="72">
+        <v>4</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="72"/>
+      <c r="E5" s="75" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F5" s="76"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="72">
+        <v>5</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+    </row>
+    <row r="7" spans="1:6" ht="60">
+      <c r="A7" s="72">
+        <v>6</v>
+      </c>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="71" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F7" s="76"/>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="72">
+        <v>7</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="75" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F8" s="76"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="72">
+        <v>8</v>
+      </c>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="72">
+        <v>9</v>
+      </c>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="76"/>
+    </row>
+    <row r="11" spans="1:6" ht="60">
+      <c r="A11" s="72">
+        <v>10</v>
+      </c>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="E11" s="75" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F11" s="76"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="72">
+        <v>11</v>
+      </c>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="75" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F12" s="76"/>
+    </row>
+    <row r="13" spans="1:6" ht="45">
+      <c r="A13" s="72">
+        <v>12</v>
+      </c>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="75" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F13" s="76"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="72">
+        <v>13</v>
+      </c>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="76"/>
+    </row>
+    <row r="15" spans="1:6" ht="75">
+      <c r="A15" s="72">
+        <v>14</v>
+      </c>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F15" s="76"/>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="72">
+        <v>15</v>
+      </c>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="75" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F16" s="76"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="72">
+        <v>16</v>
+      </c>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="76"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="72">
+        <v>17</v>
+      </c>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="76"/>
+    </row>
+    <row r="19" spans="1:6" ht="90">
+      <c r="A19" s="72">
+        <v>18</v>
+      </c>
+      <c r="B19" s="72"/>
+      <c r="C19" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="72"/>
+      <c r="E19" s="75" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F19" s="76"/>
+    </row>
+    <row r="20" spans="1:6" ht="105">
+      <c r="A20" s="72">
+        <v>19</v>
+      </c>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="75" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F20" s="76"/>
+    </row>
+    <row r="21" spans="1:6" ht="90">
+      <c r="A21" s="72">
+        <v>20</v>
+      </c>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="75" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F21" s="76"/>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="A22" s="72">
+        <v>21</v>
+      </c>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22" s="75" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F22" s="76"/>
+    </row>
+    <row r="23" spans="1:6" ht="45">
+      <c r="A23" s="72">
+        <v>22</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="75" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F23" s="76"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="72">
+        <v>23</v>
+      </c>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="76"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="72">
+        <v>24</v>
+      </c>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="76"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="72">
+        <v>25</v>
+      </c>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="76"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F26" xr:uid="{79DFBE3C-4481-4C95-B99D-8546E6AE3B3F}">
+      <formula1>"Task1, Task 2, Task3, Task 4, Task 5, Task 6, Task 7, Task 8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C26" xr:uid="{B5660EDC-ABE6-43C4-8718-E55E85DFCB39}">
+      <formula1>"English,Knowledge Gaps,Emotion,Techniques"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F1" location="'Domain-Initiating'!A1" display="Domain" xr:uid="{38E319FA-B19C-4937-88A6-EA1BC07324E4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29A3CE1-998F-4ACC-B0C1-F793A7B2A89D}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42057,7 +42464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67830A5-61CE-4324-A223-E0E1F9224A73}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G26"/>
@@ -42450,7 +42857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F5D74C-E5D9-45C3-98E4-07977C9F0161}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E11"/>
@@ -42596,7 +43003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C982353-CA8A-4388-8859-7413C89A9E50}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E26"/>
@@ -42949,7 +43356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3E4B6E-32AB-4F9F-9656-4C5398F92691}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L52"/>
@@ -43928,7 +44335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAC2793-45B1-4029-830E-35CE2386D9D1}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J51"/>
@@ -44965,7 +45372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0762741B-203C-43CC-95E6-55D0B96E24E3}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F51"/>
@@ -45667,7 +46074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C21AC00-F23C-4DDA-9EE8-A43E265F9EB8}">
   <dimension ref="A1:F51"/>
   <sheetViews>
@@ -46315,7 +46722,172 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD3A80B-5C92-444C-86E6-05BC29695160}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="68"/>
+    <col min="2" max="2" width="21.42578125" style="68" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="68" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="68" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" style="68" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="4" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="4" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="4" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="120">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="4" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="4" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="4" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="27">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="4" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75">
+      <c r="A10" s="27">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="4" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="27">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{A5DEE7C1-57C2-47E9-BB78-F7A901A4DFD7}">
+      <formula1>"English,Knowledge Gaps,Emotion,Techniques"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B485323A-E48D-48D5-A059-00902955E19C}">
   <dimension ref="A1:G51"/>
   <sheetViews>
@@ -46994,170 +47566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD3A80B-5C92-444C-86E6-05BC29695160}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="68"/>
-    <col min="2" max="2" width="21.42578125" style="68" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="68" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="68" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" style="68" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="68"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="26.25">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="27">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="27">
-        <v>2</v>
-      </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="27">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="120">
-      <c r="A5" s="27">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="4" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="27">
-        <v>5</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="4" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="27">
-        <v>6</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
-      <c r="A8" s="27">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="27">
-        <v>8</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="4" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75">
-      <c r="A10" s="27">
-        <v>9</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="4" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="27">
-        <v>10</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27" t="s">
-        <v>832</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{A5DEE7C1-57C2-47E9-BB78-F7A901A4DFD7}">
-      <formula1>"English,Knowledge Gaps,Emotion,Techniques"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574CC2A3-93D7-4AB9-83CF-AF68AB756A5A}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -47545,7 +47954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFD739-AF93-4AA7-A2F1-3E80882A8922}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F51"/>
@@ -48242,7 +48651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475F131D-CBCC-4B8F-BDF4-B1E2E34C7098}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K9"/>
@@ -48420,7 +48829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E6B415-86AF-44A1-9A0F-E640C770D3EB}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:K13"/>
@@ -48652,6 +49061,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -48659,18 +49074,12 @@
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E3A676-4755-49BB-A0B9-3FC0BA4B80B3}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K7"/>
@@ -48787,151 +49196,6 @@
       </c>
       <c r="B7" s="129" t="s">
         <v>154</v>
-      </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="131"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="B6:K6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4D9506-FE81-4C50-86CB-42DFDE5F4697}">
-  <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A1" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="129" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="131"/>
-    </row>
-    <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A2" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="129" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="131"/>
-    </row>
-    <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A3" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="129" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="131"/>
-    </row>
-    <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="129" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
-      <c r="K4" s="131"/>
-    </row>
-    <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A5" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="129" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
-      <c r="K5" s="131"/>
-    </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
-      <c r="A6" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="129" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="130"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="130"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="130"/>
-      <c r="K6" s="131"/>
-    </row>
-    <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
-      <c r="A7" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="129" t="s">
-        <v>162</v>
       </c>
       <c r="C7" s="130"/>
       <c r="D7" s="130"/>
@@ -48959,6 +49223,151 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4D9506-FE81-4C50-86CB-42DFDE5F4697}">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="129" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="131"/>
+    </row>
+    <row r="2" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="131"/>
+    </row>
+    <row r="3" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
+    </row>
+    <row r="4" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="131"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="129" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
+      <c r="K5" s="131"/>
+    </row>
+    <row r="6" spans="1:11" ht="45" customHeight="1" thickBot="1">
+      <c r="A6" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="129" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="131"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A7" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="129" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="131"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFC2900-1516-4D11-BB5E-CB91221B0668}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K8"/>
@@ -49118,7 +49527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8370EABC-5FB0-46E3-AC0D-18A12C9132DD}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:E26"/>
@@ -49405,28 +49814,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B150C828-5E38-4F9B-89F5-DE7664E9E60A}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20858FF-860F-4DDB-90C1-5CC740EF8BB8}">
-  <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49602,6 +49996,21 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20858FF-860F-4DDB-90C1-5CC740EF8BB8}">
+  <sheetPr codeName="Sheet17"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E5ACBF-E712-4A9D-9910-ED74A62FE5AE}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1"/>
@@ -49614,7 +50023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C417280C-3257-4FCE-BFBC-576DD1B4382F}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
tap trung  tap trung khong bao gio truot
</commit_message>
<xml_diff>
--- a/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
+++ b/10_Management/Exam_PMP_TangToc_07032019 - TrungLV_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\EBill\10_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D8BD8-1268-43B9-A8CB-63CB7A8110B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E6114-BBE7-404E-B319-280CB85A2E5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{957D22A2-4D54-4148-9DDE-7A2AF7FA87D7}"/>
   </bookViews>
   <sheets>
     <sheet name="study plan" sheetId="22" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="1074">
   <si>
     <t>No</t>
   </si>
@@ -2653,9 +2653,6 @@
 cost of conformance: rework, scrap, warranty work, </t>
   </si>
   <si>
-    <t>cái nào cho phép cách tiếp cận hỗ trợ việc quản lý risk mơ hồ</t>
-  </si>
-  <si>
     <t>ambiguity risk là viêc thiếu hụt (deficit) kiến thức hoặc hiểu sai dẫn đến cần có sự expert external input or bench marking against best practice</t>
   </si>
   <si>
@@ -3369,9 +3366,6 @@
     <t>Note: khi đã nhận được kết quả project charter đã approve thì việc tiếp theo cần phải thông báo cho các stakeholder. Project manager's responsibility to inform all key stakeholser of the approved project charter và ensure common understanding of the key deliverable, milestones, their roles and responsibility</t>
   </si>
   <si>
-    <t>Note: nếu contract có 1 change request bị reject sớm trong process. Bạn có thể có 1 record  như là request changes trong project's correspondence  with the customer in this case</t>
-  </si>
-  <si>
     <t>Contract FFP không nên được sử dụng trừ khi mà  scope of work và specifications được document lại chính xác. Trong trường hợp này có thể sử dụng T&amp;M Contract hoặc cost-plus nếu mà contractor có requested amendments to their contact. Trường hợp mà scope k rõ ràng nhưng lại sử dụng FFP contract thì có thể sẽ dẫn đến disputes and future claims</t>
   </si>
   <si>
@@ -3476,6 +3470,33 @@
   </si>
   <si>
     <t>Chưa làm</t>
+  </si>
+  <si>
+    <t>PMO cần điều chỉnh mục tiêu của dự án theo chiến lược của công ty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: nếu contract có 1 change request bị reject sớm trong process. Bạn có thể có 1 record  như là request changes trong project's correspondence  with the customer in this case </t>
+  </si>
+  <si>
+    <t>work performance report là output của project intergration management process</t>
+  </si>
+  <si>
+    <t>đọc lại nội dung informal và unofficial</t>
+  </si>
+  <si>
+    <t>Vấn đề đọc hiểu tiếng anh.</t>
+  </si>
+  <si>
+    <t>đọc lại discount cash flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cái nào cho phép cách tiếp cận hỗ trợ việc quản lý risk mơ hồ. </t>
+  </si>
+  <si>
+    <t>đọc lại nội dung câu project final report</t>
+  </si>
+  <si>
+    <t>xem lại</t>
   </si>
 </sst>
 </file>
@@ -4814,8 +4835,8 @@
   </sheetPr>
   <dimension ref="A1:AA1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -4846,7 +4867,7 @@
         <v>575</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H1" s="60" t="s">
         <v>459</v>
@@ -5902,7 +5923,7 @@
         <v>480</v>
       </c>
       <c r="I26" s="98" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="J26" s="56"/>
       <c r="K26" s="56"/>
@@ -6008,7 +6029,7 @@
     </row>
     <row r="29" spans="1:27" ht="15">
       <c r="A29" s="121" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B29" s="122">
         <v>43499</v>
@@ -6157,7 +6178,7 @@
         <v>480</v>
       </c>
       <c r="I32" s="112" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="J32" s="56"/>
       <c r="K32" s="56"/>
@@ -6180,7 +6201,7 @@
     </row>
     <row r="33" spans="1:27" ht="15">
       <c r="A33" s="121" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B33" s="122">
         <f>B30+ 1</f>
@@ -6307,7 +6328,7 @@
     </row>
     <row r="36" spans="1:27" ht="15">
       <c r="A36" s="125" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B36" s="122">
         <f>B30 + 10</f>
@@ -6436,7 +6457,7 @@
     </row>
     <row r="39" spans="1:27" ht="15">
       <c r="A39" s="125" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B39" s="122">
         <f t="shared" si="6"/>
@@ -6565,7 +6586,7 @@
     </row>
     <row r="42" spans="1:27" ht="15">
       <c r="A42" s="125" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B42" s="122">
         <f t="shared" si="6"/>
@@ -6692,7 +6713,7 @@
     </row>
     <row r="45" spans="1:27" ht="15">
       <c r="A45" s="125" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B45" s="122">
         <f>B38+ 2</f>
@@ -6817,7 +6838,7 @@
     </row>
     <row r="48" spans="1:27" ht="15">
       <c r="A48" s="125" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B48" s="122">
         <f>B45+1</f>
@@ -6938,7 +6959,7 @@
     </row>
     <row r="51" spans="1:27" ht="15">
       <c r="A51" s="125" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B51" s="122">
         <f>B45 + 2</f>
@@ -6992,7 +7013,7 @@
       </c>
       <c r="E52" s="110"/>
       <c r="F52" s="111" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="G52" s="111"/>
       <c r="H52" s="111"/>
@@ -7059,7 +7080,7 @@
     </row>
     <row r="54" spans="1:27" ht="15">
       <c r="A54" s="125" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B54" s="122">
         <f>B45+3</f>
@@ -7180,7 +7201,7 @@
     </row>
     <row r="57" spans="1:27" ht="15">
       <c r="A57" s="125" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B57" s="122">
         <f t="shared" si="9"/>
@@ -7297,7 +7318,7 @@
     </row>
     <row r="60" spans="1:27" ht="15">
       <c r="A60" s="125" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B60" s="122">
         <f t="shared" si="9"/>
@@ -31659,7 +31680,7 @@
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
       <c r="E2" s="72" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F2" s="27"/>
     </row>
@@ -31671,7 +31692,7 @@
       <c r="C3" s="72"/>
       <c r="D3" s="72"/>
       <c r="E3" s="72" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="F3" s="27"/>
     </row>
@@ -31695,7 +31716,7 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="4" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F5" s="27"/>
     </row>
@@ -31709,7 +31730,7 @@
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F6" s="27"/>
     </row>
@@ -31721,7 +31742,7 @@
       <c r="C7" s="27"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="88"/>
@@ -31756,7 +31777,7 @@
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F10" s="89"/>
       <c r="G10" s="88"/>
@@ -31834,7 +31855,7 @@
       </c>
       <c r="D2" s="72"/>
       <c r="E2" s="75" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F2" s="68" t="s">
         <v>515</v>
@@ -31866,7 +31887,7 @@
         <v>518</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>515</v>
@@ -31879,14 +31900,14 @@
       <c r="B5" s="72"/>
       <c r="C5" s="72"/>
       <c r="D5" s="72" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E5" s="75" t="e">
         <f>- It must be noted that the car has been built, and the Control Quality and Validate Scope processes have been performed for every deliverable. the question is asking about PRODUCT delivery, which occurs during the closing process</f>
         <v>#NAME?</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -31926,7 +31947,7 @@
       </c>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F8" s="81" t="s">
         <v>523</v>
@@ -31998,7 +32019,7 @@
       </c>
       <c r="D13" s="72"/>
       <c r="E13" s="75" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F13" s="81"/>
     </row>
@@ -32082,7 +32103,7 @@
       </c>
       <c r="D19" s="72"/>
       <c r="E19" s="75" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F19" s="82" t="s">
         <v>536</v>
@@ -32112,10 +32133,10 @@
         <v>538</v>
       </c>
       <c r="E21" s="75" t="s">
+        <v>909</v>
+      </c>
+      <c r="F21" s="68" t="s">
         <v>910</v>
-      </c>
-      <c r="F21" s="68" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -32140,7 +32161,7 @@
       <c r="C23" s="72"/>
       <c r="D23" s="72"/>
       <c r="E23" s="75" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -32151,7 +32172,7 @@
       <c r="C24" s="72"/>
       <c r="D24" s="72"/>
       <c r="E24" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -32171,7 +32192,7 @@
       <c r="C26" s="72"/>
       <c r="D26" s="72"/>
       <c r="E26" s="75" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -32201,7 +32222,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="72" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E29" s="75"/>
     </row>
@@ -32233,7 +32254,7 @@
       </c>
       <c r="D32" s="72"/>
       <c r="E32" s="75" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -32263,10 +32284,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="72" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -32279,7 +32300,7 @@
       </c>
       <c r="D36" s="72"/>
       <c r="E36" s="75" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -32290,7 +32311,7 @@
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
       <c r="E37" s="75" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -32303,7 +32324,7 @@
       </c>
       <c r="D38" s="72"/>
       <c r="E38" s="75" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -32315,7 +32336,7 @@
         <v>4</v>
       </c>
       <c r="D39" s="72" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E39" s="75"/>
     </row>
@@ -32337,7 +32358,7 @@
         <v>4</v>
       </c>
       <c r="D41" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E41" s="75"/>
     </row>
@@ -32350,7 +32371,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="72" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E42" s="75"/>
     </row>
@@ -32363,7 +32384,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="72" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E43" s="75"/>
     </row>
@@ -32403,7 +32424,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="72" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E47" s="75"/>
     </row>
@@ -33079,8 +33100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD440D0-468F-462B-9532-3FA36BB45DDC}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D44" activeCellId="1" sqref="E46 D44"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33151,7 +33172,7 @@
       </c>
       <c r="D5" s="72"/>
       <c r="E5" s="75" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75">
@@ -33164,7 +33185,7 @@
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="75" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45">
@@ -33175,7 +33196,7 @@
       <c r="C7" s="72"/>
       <c r="D7" s="72"/>
       <c r="E7" s="75" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="G7" s="77"/>
     </row>
@@ -33198,7 +33219,7 @@
       </c>
       <c r="D9" s="72"/>
       <c r="E9" s="75" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -33228,7 +33249,7 @@
       <c r="C12" s="72"/>
       <c r="D12" s="72"/>
       <c r="E12" s="75" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -33250,7 +33271,7 @@
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="75" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -33270,7 +33291,7 @@
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
       <c r="E16" s="75" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="105">
@@ -33283,7 +33304,7 @@
       </c>
       <c r="D17" s="72"/>
       <c r="E17" s="75" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -33295,14 +33316,16 @@
       <c r="D18" s="72"/>
       <c r="E18" s="75"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="30">
       <c r="A19" s="72">
         <v>18</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="72"/>
       <c r="D19" s="72"/>
-      <c r="E19" s="75"/>
+      <c r="E19" s="75" t="s">
+        <v>1065</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="72">
@@ -33321,9 +33344,11 @@
       <c r="C21" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="72"/>
+      <c r="D21" s="72" t="s">
+        <v>76</v>
+      </c>
       <c r="E21" s="75" t="s">
-        <v>1031</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -33354,7 +33379,7 @@
       </c>
       <c r="D24" s="72"/>
       <c r="E24" s="75" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45">
@@ -33367,7 +33392,7 @@
       </c>
       <c r="D25" s="72"/>
       <c r="E25" s="75" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60">
@@ -33378,9 +33403,11 @@
       <c r="C26" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="72"/>
+      <c r="D26" s="72" t="s">
+        <v>1067</v>
+      </c>
       <c r="E26" s="75" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45">
@@ -33391,7 +33418,7 @@
       <c r="C27" s="72"/>
       <c r="D27" s="72"/>
       <c r="E27" s="75" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45">
@@ -33402,7 +33429,7 @@
       <c r="C28" s="72"/>
       <c r="D28" s="72"/>
       <c r="E28" s="75" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -33422,7 +33449,7 @@
       <c r="C30" s="72"/>
       <c r="D30" s="72"/>
       <c r="E30" s="75" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -33471,7 +33498,7 @@
       </c>
       <c r="D35" s="72"/>
       <c r="E35" s="75" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45">
@@ -33484,7 +33511,7 @@
       </c>
       <c r="D36" s="72"/>
       <c r="E36" s="75" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30">
@@ -33495,9 +33522,11 @@
       <c r="C37" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="72"/>
+      <c r="D37" s="72" t="s">
+        <v>1068</v>
+      </c>
       <c r="E37" s="75" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="60">
@@ -33510,7 +33539,7 @@
       </c>
       <c r="D38" s="72"/>
       <c r="E38" s="75" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="120">
@@ -33523,7 +33552,7 @@
       </c>
       <c r="D39" s="72"/>
       <c r="E39" s="75" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30">
@@ -33534,9 +33563,11 @@
       <c r="C40" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="72"/>
+      <c r="D40" s="72" t="s">
+        <v>1069</v>
+      </c>
       <c r="E40" s="75" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -33558,7 +33589,7 @@
       </c>
       <c r="D42" s="72"/>
       <c r="E42" s="75" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="105">
@@ -33569,9 +33600,11 @@
       <c r="C43" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="72"/>
+      <c r="D43" s="72" t="s">
+        <v>1070</v>
+      </c>
       <c r="E43" s="75" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -33613,7 +33646,7 @@
       </c>
       <c r="D47" s="72"/>
       <c r="E47" s="75" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="45">
@@ -33626,7 +33659,7 @@
       </c>
       <c r="D48" s="72"/>
       <c r="E48" s="75" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="105">
@@ -33638,10 +33671,10 @@
         <v>4</v>
       </c>
       <c r="D49" s="72" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="60">
@@ -33654,7 +33687,7 @@
       </c>
       <c r="D50" s="72"/>
       <c r="E50" s="75" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="120">
@@ -33666,10 +33699,10 @@
         <v>4</v>
       </c>
       <c r="D51" s="72" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E51" s="75" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
@@ -35585,7 +35618,7 @@
       </c>
       <c r="D2" s="72"/>
       <c r="E2" s="75" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F2" s="76"/>
     </row>
@@ -35599,7 +35632,7 @@
       </c>
       <c r="D3" s="72"/>
       <c r="E3" s="75" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F3" s="76"/>
     </row>
@@ -35621,7 +35654,7 @@
       <c r="C5" s="72"/>
       <c r="D5" s="72"/>
       <c r="E5" s="75" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F5" s="76"/>
     </row>
@@ -35633,7 +35666,7 @@
       <c r="C6" s="72"/>
       <c r="D6" s="72"/>
       <c r="E6" s="75" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F6" s="76"/>
     </row>
@@ -35646,10 +35679,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="72" t="s">
+        <v>948</v>
+      </c>
+      <c r="E7" s="75" t="s">
         <v>949</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>950</v>
       </c>
       <c r="F7" s="76"/>
       <c r="G7" s="77"/>
@@ -35664,7 +35697,7 @@
       </c>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -35676,7 +35709,7 @@
       <c r="C9" s="72"/>
       <c r="D9" s="72"/>
       <c r="E9" s="75" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F9" s="76"/>
     </row>
@@ -35711,10 +35744,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="72" t="s">
+        <v>952</v>
+      </c>
+      <c r="E12" s="75" t="s">
         <v>953</v>
-      </c>
-      <c r="E12" s="75" t="s">
-        <v>954</v>
       </c>
       <c r="F12" s="76"/>
     </row>
@@ -35778,7 +35811,7 @@
       </c>
       <c r="D18" s="72"/>
       <c r="E18" s="75" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F18" s="76"/>
     </row>
@@ -35812,7 +35845,7 @@
       </c>
       <c r="D21" s="72"/>
       <c r="E21" s="75" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F21" s="76"/>
     </row>
@@ -35846,7 +35879,7 @@
       </c>
       <c r="D24" s="72"/>
       <c r="E24" s="75" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F24" s="76"/>
     </row>
@@ -35857,7 +35890,7 @@
       <c r="B25" s="72"/>
       <c r="C25" s="72"/>
       <c r="D25" s="72" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E25" s="75"/>
       <c r="F25" s="76"/>
@@ -35880,7 +35913,7 @@
       <c r="C27" s="72"/>
       <c r="D27" s="72"/>
       <c r="E27" s="75" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F27" s="76"/>
     </row>
@@ -35894,7 +35927,7 @@
       </c>
       <c r="D28" s="72"/>
       <c r="E28" s="75" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F28" s="76"/>
     </row>
@@ -35908,7 +35941,7 @@
       </c>
       <c r="D29" s="72"/>
       <c r="E29" s="75" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F29" s="76"/>
     </row>
@@ -35920,7 +35953,7 @@
       <c r="C30" s="72"/>
       <c r="D30" s="72"/>
       <c r="E30" s="75" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F30" s="76"/>
     </row>
@@ -35944,7 +35977,7 @@
       </c>
       <c r="D32" s="72"/>
       <c r="E32" s="75" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F32" s="76"/>
     </row>
@@ -35956,7 +35989,7 @@
       <c r="C33" s="72"/>
       <c r="D33" s="72"/>
       <c r="E33" s="75" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F33" s="76"/>
     </row>
@@ -35970,7 +36003,7 @@
       </c>
       <c r="D34" s="72"/>
       <c r="E34" s="75" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F34" s="76"/>
     </row>
@@ -35994,7 +36027,7 @@
       </c>
       <c r="D36" s="72"/>
       <c r="E36" s="75" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="F36" s="76"/>
     </row>
@@ -36038,7 +36071,7 @@
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="75" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="F40" s="76"/>
     </row>
@@ -36051,7 +36084,7 @@
         <v>4</v>
       </c>
       <c r="D41" s="72" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E41" s="75"/>
       <c r="F41" s="76"/>
@@ -36066,7 +36099,7 @@
       </c>
       <c r="D42" s="72"/>
       <c r="E42" s="75" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F42" s="76"/>
     </row>
@@ -36080,7 +36113,7 @@
       </c>
       <c r="D43" s="72"/>
       <c r="E43" s="75" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F43" s="76"/>
     </row>
@@ -36094,7 +36127,7 @@
       </c>
       <c r="D44" s="72"/>
       <c r="E44" s="75" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F44" s="76"/>
     </row>
@@ -36108,7 +36141,7 @@
       </c>
       <c r="D45" s="72"/>
       <c r="E45" s="75" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F45" s="76"/>
     </row>
@@ -36141,7 +36174,7 @@
       </c>
       <c r="D48" s="72"/>
       <c r="E48" s="75" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F48" s="76"/>
     </row>
@@ -36155,7 +36188,7 @@
       </c>
       <c r="D49" s="72"/>
       <c r="E49" s="75" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F49" s="76"/>
     </row>
@@ -36169,7 +36202,7 @@
       </c>
       <c r="D50" s="72"/>
       <c r="E50" s="75" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F50" s="76"/>
     </row>
@@ -36183,7 +36216,7 @@
       </c>
       <c r="D51" s="72"/>
       <c r="E51" s="75" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F51" s="76"/>
     </row>
@@ -36248,7 +36281,7 @@
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
       <c r="E2" s="75" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F2" s="76"/>
     </row>
@@ -36272,7 +36305,7 @@
       </c>
       <c r="D4" s="72"/>
       <c r="E4" s="75" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F4" s="76"/>
     </row>
@@ -36296,7 +36329,7 @@
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="75" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F6" s="76"/>
     </row>
@@ -36310,7 +36343,7 @@
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="75" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F7" s="76"/>
       <c r="G7" s="77"/>
@@ -36325,7 +36358,7 @@
       </c>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -36391,7 +36424,7 @@
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="75" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="F14" s="76"/>
     </row>
@@ -36413,7 +36446,7 @@
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
       <c r="E16" s="75" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F16" s="76"/>
     </row>
@@ -36425,7 +36458,7 @@
       <c r="C17" s="72"/>
       <c r="D17" s="72"/>
       <c r="E17" s="75" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F17" s="76"/>
     </row>
@@ -36437,7 +36470,7 @@
       <c r="C18" s="72"/>
       <c r="D18" s="72"/>
       <c r="E18" s="75" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F18" s="76"/>
     </row>
@@ -36449,7 +36482,7 @@
       <c r="C19" s="72"/>
       <c r="D19" s="72"/>
       <c r="E19" s="75" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F19" s="76"/>
     </row>
@@ -36471,7 +36504,7 @@
       <c r="C21" s="72"/>
       <c r="D21" s="72"/>
       <c r="E21" s="75" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F21" s="76"/>
     </row>
@@ -36483,7 +36516,7 @@
       <c r="C22" s="72"/>
       <c r="D22" s="72"/>
       <c r="E22" s="75" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F22" s="76"/>
     </row>
@@ -36497,7 +36530,7 @@
       </c>
       <c r="D23" s="72"/>
       <c r="E23" s="75" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F23" s="76"/>
     </row>
@@ -36511,7 +36544,7 @@
       </c>
       <c r="D24" s="72"/>
       <c r="E24" s="75" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F24" s="76"/>
     </row>
@@ -36535,7 +36568,7 @@
       </c>
       <c r="D26" s="72"/>
       <c r="E26" s="75" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F26" s="76"/>
     </row>
@@ -36549,7 +36582,7 @@
       </c>
       <c r="D27" s="72"/>
       <c r="E27" s="75" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F27" s="76"/>
     </row>
@@ -36573,7 +36606,7 @@
       </c>
       <c r="D29" s="72"/>
       <c r="E29" s="75" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F29" s="76"/>
     </row>
@@ -36587,7 +36620,7 @@
       </c>
       <c r="D30" s="72"/>
       <c r="E30" s="75" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F30" s="76"/>
     </row>
@@ -36611,7 +36644,7 @@
       </c>
       <c r="D32" s="72"/>
       <c r="E32" s="75" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F32" s="76"/>
     </row>
@@ -36637,7 +36670,7 @@
       </c>
       <c r="D34" s="72"/>
       <c r="E34" s="75" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F34" s="76"/>
     </row>
@@ -36671,7 +36704,7 @@
       </c>
       <c r="D37" s="72"/>
       <c r="E37" s="75" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F37" s="76"/>
     </row>
@@ -36692,10 +36725,10 @@
       <c r="B39" s="72"/>
       <c r="C39" s="72"/>
       <c r="D39" s="72" t="s">
+        <v>934</v>
+      </c>
+      <c r="E39" s="75" t="s">
         <v>935</v>
-      </c>
-      <c r="E39" s="75" t="s">
-        <v>936</v>
       </c>
       <c r="F39" s="76"/>
     </row>
@@ -36709,7 +36742,7 @@
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="75" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F40" s="76"/>
     </row>
@@ -36723,7 +36756,7 @@
       </c>
       <c r="D41" s="72"/>
       <c r="E41" s="75" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F41" s="76"/>
     </row>
@@ -36735,7 +36768,7 @@
       <c r="C42" s="72"/>
       <c r="D42" s="72"/>
       <c r="E42" s="75" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F42" s="76"/>
     </row>
@@ -36769,7 +36802,7 @@
       </c>
       <c r="D45" s="72"/>
       <c r="E45" s="75" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F45" s="76"/>
     </row>
@@ -36783,7 +36816,7 @@
       </c>
       <c r="D46" s="72"/>
       <c r="E46" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F46" s="76"/>
     </row>
@@ -36804,7 +36837,7 @@
       <c r="C48" s="72"/>
       <c r="D48" s="72"/>
       <c r="E48" s="75" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F48" s="76"/>
     </row>
@@ -36818,7 +36851,7 @@
       </c>
       <c r="D49" s="72"/>
       <c r="E49" s="75" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F49" s="76"/>
     </row>
@@ -36830,7 +36863,7 @@
       <c r="C50" s="72"/>
       <c r="D50" s="72"/>
       <c r="E50" s="75" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F50" s="76"/>
     </row>
@@ -37423,7 +37456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03EE777-7A71-4ABF-B428-9DD9FC79554D}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -37724,10 +37759,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="72" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E21" s="75" t="s">
         <v>797</v>
-      </c>
-      <c r="E21" s="75" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -37756,7 +37791,7 @@
       <c r="C24" s="72"/>
       <c r="D24" s="72"/>
       <c r="E24" s="75" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30">
@@ -37769,7 +37804,7 @@
       </c>
       <c r="D25" s="72"/>
       <c r="E25" s="75" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45">
@@ -37782,10 +37817,10 @@
       </c>
       <c r="D26" s="72"/>
       <c r="E26" s="75" t="s">
+        <v>800</v>
+      </c>
+      <c r="F26" s="68" t="s">
         <v>801</v>
-      </c>
-      <c r="F26" s="68" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="75">
@@ -37796,9 +37831,11 @@
       <c r="C27" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="72"/>
+      <c r="D27" s="72" t="s">
+        <v>1072</v>
+      </c>
       <c r="E27" s="75" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="45">
@@ -37809,7 +37846,7 @@
       <c r="C28" s="72"/>
       <c r="D28" s="72"/>
       <c r="E28" s="75" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30">
@@ -37822,7 +37859,7 @@
       </c>
       <c r="D29" s="72"/>
       <c r="E29" s="75" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -37844,10 +37881,10 @@
       </c>
       <c r="D31" s="72"/>
       <c r="E31" s="75" t="s">
+        <v>805</v>
+      </c>
+      <c r="F31" s="68" t="s">
         <v>806</v>
-      </c>
-      <c r="F31" s="68" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90">
@@ -37860,7 +37897,7 @@
       </c>
       <c r="D32" s="72"/>
       <c r="E32" s="75" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F32" s="68" t="s">
         <v>554</v>
@@ -37874,7 +37911,7 @@
       <c r="C33" s="72"/>
       <c r="D33" s="72"/>
       <c r="E33" s="75" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="60">
@@ -37885,7 +37922,7 @@
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
       <c r="E34" s="75" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -37898,7 +37935,7 @@
       </c>
       <c r="D35" s="72"/>
       <c r="E35" s="75" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -37916,7 +37953,9 @@
       </c>
       <c r="B37" s="72"/>
       <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
+      <c r="D37" s="72" t="s">
+        <v>1073</v>
+      </c>
       <c r="E37" s="75"/>
     </row>
     <row r="38" spans="1:6" ht="45">
@@ -37927,10 +37966,10 @@
       <c r="C38" s="72"/>
       <c r="D38" s="72"/>
       <c r="E38" s="75" t="s">
+        <v>811</v>
+      </c>
+      <c r="F38" s="68" t="s">
         <v>812</v>
-      </c>
-      <c r="F38" s="68" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="45">
@@ -37943,7 +37982,7 @@
       </c>
       <c r="D39" s="72"/>
       <c r="E39" s="75" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -37965,7 +38004,7 @@
       </c>
       <c r="D41" s="72"/>
       <c r="E41" s="75" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -37987,10 +38026,10 @@
       </c>
       <c r="D43" s="72"/>
       <c r="E43" s="75" t="s">
+        <v>815</v>
+      </c>
+      <c r="F43" s="68" t="s">
         <v>816</v>
-      </c>
-      <c r="F43" s="68" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -38011,10 +38050,10 @@
         <v>4</v>
       </c>
       <c r="D45" s="72" t="s">
+        <v>817</v>
+      </c>
+      <c r="E45" s="75" t="s">
         <v>818</v>
-      </c>
-      <c r="E45" s="75" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="45">
@@ -38025,7 +38064,7 @@
       <c r="C46" s="72"/>
       <c r="D46" s="72"/>
       <c r="E46" s="75" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="75">
@@ -38036,7 +38075,7 @@
       <c r="C47" s="72"/>
       <c r="D47" s="72"/>
       <c r="E47" s="75" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30">
@@ -38047,7 +38086,7 @@
       <c r="C48" s="72"/>
       <c r="D48" s="72"/>
       <c r="E48" s="75" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -40039,7 +40078,7 @@
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60">
@@ -40052,7 +40091,7 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -40090,7 +40129,7 @@
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="90">
@@ -40101,7 +40140,7 @@
       <c r="C8" s="27"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="105">
@@ -40112,7 +40151,7 @@
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="105">
@@ -40123,7 +40162,7 @@
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
       <c r="E10" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="150">
@@ -40134,7 +40173,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
   </sheetData>
@@ -40190,7 +40229,7 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -40219,7 +40258,7 @@
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -40239,7 +40278,7 @@
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -40277,7 +40316,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -41851,7 +41890,7 @@
       </c>
       <c r="D5" s="72"/>
       <c r="E5" s="75" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="F5" s="76"/>
     </row>
@@ -41875,7 +41914,7 @@
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="71" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="F7" s="76"/>
     </row>
@@ -41887,7 +41926,7 @@
       <c r="C8" s="72"/>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -41921,7 +41960,7 @@
       </c>
       <c r="D11" s="72"/>
       <c r="E11" s="75" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="F11" s="76"/>
     </row>
@@ -41933,7 +41972,7 @@
       <c r="C12" s="72"/>
       <c r="D12" s="72"/>
       <c r="E12" s="75" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="F12" s="76"/>
     </row>
@@ -41947,7 +41986,7 @@
       </c>
       <c r="D13" s="72"/>
       <c r="E13" s="75" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="F13" s="76"/>
     </row>
@@ -41970,7 +42009,7 @@
       </c>
       <c r="D15" s="72"/>
       <c r="E15" s="72" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="F15" s="76"/>
     </row>
@@ -41982,7 +42021,7 @@
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
       <c r="E16" s="75" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="F16" s="76"/>
     </row>
@@ -42016,7 +42055,7 @@
       </c>
       <c r="D19" s="72"/>
       <c r="E19" s="75" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="F19" s="76"/>
     </row>
@@ -42028,7 +42067,7 @@
       <c r="C20" s="72"/>
       <c r="D20" s="72"/>
       <c r="E20" s="75" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="F20" s="76"/>
     </row>
@@ -42040,7 +42079,7 @@
       <c r="C21" s="72"/>
       <c r="D21" s="72"/>
       <c r="E21" s="75" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="F21" s="76"/>
     </row>
@@ -42054,7 +42093,7 @@
       </c>
       <c r="D22" s="72"/>
       <c r="E22" s="75" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="F22" s="76"/>
     </row>
@@ -42066,7 +42105,7 @@
       <c r="C23" s="72"/>
       <c r="D23" s="72"/>
       <c r="E23" s="75" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="F23" s="76"/>
     </row>
@@ -42165,7 +42204,7 @@
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
       <c r="E2" s="75" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F2" s="76"/>
     </row>
@@ -42177,7 +42216,7 @@
       <c r="C3" s="72"/>
       <c r="D3" s="72"/>
       <c r="E3" s="75" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F3" s="76"/>
     </row>
@@ -42189,7 +42228,7 @@
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
       <c r="E4" s="75" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F4" s="76"/>
     </row>
@@ -42201,7 +42240,7 @@
       <c r="C5" s="72"/>
       <c r="D5" s="72"/>
       <c r="E5" s="75" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F5" s="76"/>
     </row>
@@ -42225,7 +42264,7 @@
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="71" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F7" s="76"/>
     </row>
@@ -42237,7 +42276,7 @@
       <c r="C8" s="72"/>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -42261,7 +42300,7 @@
       </c>
       <c r="D10" s="72"/>
       <c r="E10" s="75" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F10" s="76"/>
     </row>
@@ -42285,7 +42324,7 @@
       </c>
       <c r="D12" s="72"/>
       <c r="E12" s="75" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F12" s="76"/>
     </row>
@@ -42297,7 +42336,7 @@
       <c r="C13" s="72"/>
       <c r="D13" s="72"/>
       <c r="E13" s="75" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F13" s="76"/>
     </row>
@@ -42308,7 +42347,7 @@
       <c r="B14" s="72"/>
       <c r="C14" s="72"/>
       <c r="E14" s="72" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F14" s="76"/>
     </row>
@@ -42322,7 +42361,7 @@
       </c>
       <c r="D15" s="72"/>
       <c r="E15" s="72" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F15" s="76"/>
     </row>
@@ -42365,10 +42404,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="72" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E19" s="75" t="s">
         <v>1019</v>
-      </c>
-      <c r="E19" s="75" t="s">
-        <v>1020</v>
       </c>
       <c r="F19" s="76"/>
     </row>
@@ -42382,7 +42421,7 @@
       </c>
       <c r="D20" s="72"/>
       <c r="E20" s="75" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F20" s="76"/>
     </row>
@@ -42416,7 +42455,7 @@
       </c>
       <c r="D23" s="72"/>
       <c r="E23" s="75" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F23" s="76"/>
     </row>
@@ -42904,7 +42943,7 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90">
@@ -42915,7 +42954,7 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -42953,7 +42992,7 @@
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -42973,7 +43012,7 @@
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -42993,7 +43032,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
   </sheetData>
@@ -46132,10 +46171,10 @@
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
       <c r="D3" s="72" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E3" s="75" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F3" s="76"/>
     </row>
@@ -46177,7 +46216,7 @@
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="75" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F7" s="76"/>
     </row>
@@ -46189,7 +46228,7 @@
       <c r="C8" s="72"/>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -46201,7 +46240,7 @@
       <c r="C9" s="72"/>
       <c r="D9" s="72"/>
       <c r="E9" s="75" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F9" s="76"/>
     </row>
@@ -46225,7 +46264,7 @@
       </c>
       <c r="D11" s="72"/>
       <c r="E11" s="75" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F11" s="76"/>
     </row>
@@ -46239,7 +46278,7 @@
       </c>
       <c r="D12" s="72"/>
       <c r="E12" s="75" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F12" s="76"/>
     </row>
@@ -46282,7 +46321,7 @@
       </c>
       <c r="D16" s="72"/>
       <c r="E16" s="75" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F16" s="76"/>
     </row>
@@ -46294,7 +46333,7 @@
       <c r="C17" s="72"/>
       <c r="D17" s="72"/>
       <c r="E17" s="75" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F17" s="76"/>
     </row>
@@ -46308,7 +46347,7 @@
       </c>
       <c r="D18" s="72"/>
       <c r="E18" s="75" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F18" s="76"/>
     </row>
@@ -46332,7 +46371,7 @@
       </c>
       <c r="D20" s="72"/>
       <c r="E20" s="75" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F20" s="76"/>
     </row>
@@ -46346,7 +46385,7 @@
       </c>
       <c r="D21" s="72"/>
       <c r="E21" s="75" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F21" s="76"/>
     </row>
@@ -46360,7 +46399,7 @@
       </c>
       <c r="D22" s="72"/>
       <c r="E22" s="75" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F22" s="76"/>
     </row>
@@ -46394,7 +46433,7 @@
       </c>
       <c r="D25" s="72"/>
       <c r="E25" s="75" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F25" s="76"/>
     </row>
@@ -46408,7 +46447,7 @@
       </c>
       <c r="D26" s="72"/>
       <c r="E26" s="75" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F26" s="76"/>
     </row>
@@ -46420,7 +46459,7 @@
       <c r="C27" s="72"/>
       <c r="D27" s="72"/>
       <c r="E27" s="75" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F27" s="76"/>
     </row>
@@ -46432,7 +46471,7 @@
       <c r="C28" s="72"/>
       <c r="D28" s="72"/>
       <c r="E28" s="75" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F28" s="76"/>
     </row>
@@ -46446,7 +46485,7 @@
       </c>
       <c r="D29" s="72"/>
       <c r="E29" s="75" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F29" s="76"/>
     </row>
@@ -46468,7 +46507,7 @@
       <c r="C31" s="72"/>
       <c r="D31" s="72"/>
       <c r="E31" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F31" s="76"/>
     </row>
@@ -46482,7 +46521,7 @@
       </c>
       <c r="D32" s="72"/>
       <c r="E32" s="75" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F32" s="76"/>
     </row>
@@ -46545,7 +46584,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="72" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E38" s="75"/>
       <c r="F38" s="76"/>
@@ -46560,7 +46599,7 @@
       </c>
       <c r="D39" s="72"/>
       <c r="E39" s="75" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F39" s="76"/>
     </row>
@@ -46574,7 +46613,7 @@
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="75" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F40" s="76"/>
     </row>
@@ -46588,7 +46627,7 @@
       </c>
       <c r="D41" s="72"/>
       <c r="E41" s="75" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="F41" s="76"/>
     </row>
@@ -46610,7 +46649,7 @@
       <c r="C43" s="72"/>
       <c r="D43" s="72"/>
       <c r="E43" s="75" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F43" s="76"/>
     </row>
@@ -46622,7 +46661,7 @@
       <c r="C44" s="72"/>
       <c r="D44" s="72"/>
       <c r="E44" s="75" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F44" s="76"/>
     </row>
@@ -46634,7 +46673,7 @@
       <c r="C45" s="72"/>
       <c r="D45" s="72"/>
       <c r="E45" s="75" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F45" s="76"/>
     </row>
@@ -46668,7 +46707,7 @@
       </c>
       <c r="D48" s="72"/>
       <c r="E48" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F48" s="76"/>
     </row>
@@ -46680,7 +46719,7 @@
       <c r="C49" s="72"/>
       <c r="D49" s="72"/>
       <c r="E49" s="75" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F49" s="76"/>
     </row>
@@ -46692,7 +46731,7 @@
       <c r="C50" s="72"/>
       <c r="D50" s="72"/>
       <c r="E50" s="75" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F50" s="76"/>
     </row>
@@ -46704,7 +46743,7 @@
       <c r="C51" s="72"/>
       <c r="D51" s="72"/>
       <c r="E51" s="75" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F51" s="76"/>
     </row>
@@ -46768,7 +46807,7 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60">
@@ -46779,7 +46818,7 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="4" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
@@ -46790,7 +46829,7 @@
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="4" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="120">
@@ -46803,7 +46842,7 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="4" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -46816,7 +46855,7 @@
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="4" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
@@ -46829,7 +46868,7 @@
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45">
@@ -46840,7 +46879,7 @@
       <c r="C8" s="27"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
@@ -46853,7 +46892,7 @@
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75">
@@ -46866,7 +46905,7 @@
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
@@ -46877,7 +46916,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
   </sheetData>
@@ -47615,7 +47654,7 @@
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
       <c r="E2" s="75" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F2" s="76"/>
     </row>
@@ -47627,7 +47666,7 @@
       <c r="C3" s="72"/>
       <c r="D3" s="72"/>
       <c r="E3" s="75" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F3" s="76"/>
     </row>
@@ -47651,11 +47690,11 @@
       </c>
       <c r="D5" s="72"/>
       <c r="E5" s="75" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F5" s="76"/>
       <c r="G5" s="71" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="165">
@@ -47670,7 +47709,7 @@
         <v>688</v>
       </c>
       <c r="E6" s="75" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F6" s="76"/>
       <c r="G6" s="71" t="s">
@@ -47687,7 +47726,7 @@
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="75" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F7" s="76"/>
     </row>
@@ -47699,7 +47738,7 @@
       <c r="C8" s="72"/>
       <c r="D8" s="72"/>
       <c r="E8" s="75" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F8" s="76"/>
     </row>
@@ -47711,7 +47750,7 @@
       <c r="C9" s="72"/>
       <c r="D9" s="72"/>
       <c r="E9" s="75" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F9" s="76"/>
     </row>
@@ -47724,10 +47763,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="72" t="s">
+        <v>840</v>
+      </c>
+      <c r="E10" s="75" t="s">
         <v>841</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>842</v>
       </c>
       <c r="F10" s="76"/>
     </row>
@@ -47741,7 +47780,7 @@
       </c>
       <c r="D11" s="72"/>
       <c r="E11" s="75" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F11" s="76"/>
     </row>
@@ -47753,7 +47792,7 @@
       <c r="C12" s="72"/>
       <c r="D12" s="72"/>
       <c r="E12" s="75" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F12" s="76"/>
     </row>
@@ -47766,14 +47805,14 @@
         <v>4</v>
       </c>
       <c r="D13" s="72" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E13" s="75" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F13" s="76"/>
       <c r="G13" s="71" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75">
@@ -47786,7 +47825,7 @@
       </c>
       <c r="D14" s="72"/>
       <c r="E14" s="75" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F14" s="76"/>
       <c r="G14" s="71" t="s">
@@ -47803,7 +47842,7 @@
       </c>
       <c r="D15" s="72"/>
       <c r="E15" s="75" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F15" s="76"/>
     </row>
@@ -47815,7 +47854,7 @@
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
       <c r="E16" s="75" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F16" s="76"/>
     </row>
@@ -47829,7 +47868,7 @@
       </c>
       <c r="D17" s="72"/>
       <c r="E17" s="75" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F17" s="76"/>
     </row>
@@ -47883,7 +47922,7 @@
       </c>
       <c r="D22" s="72"/>
       <c r="E22" s="75" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F22" s="76"/>
     </row>
@@ -47906,12 +47945,12 @@
         <v>4</v>
       </c>
       <c r="D24" s="72" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E24" s="75"/>
       <c r="F24" s="76"/>
       <c r="G24" s="71" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45">
@@ -47923,7 +47962,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="72" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E25" s="75"/>
       <c r="F25" s="76"/>
@@ -47936,7 +47975,7 @@
       <c r="C26" s="72"/>
       <c r="D26" s="72"/>
       <c r="E26" s="75" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F26" s="76"/>
     </row>
@@ -49064,6 +49103,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -49071,12 +49116,6 @@
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50242,10 +50281,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>879</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>880</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
@@ -50258,7 +50297,7 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="4" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -50278,7 +50317,7 @@
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="4" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -50336,7 +50375,7 @@
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>